<commit_message>
feedbacks, conditions des hexagones
</commit_message>
<xml_diff>
--- a/data/solutre_hex_inst.xlsx
+++ b/data/solutre_hex_inst.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="206">
   <si>
     <t>id</t>
   </si>
@@ -73,10 +73,13 @@
     <t>conditionAdjacence</t>
   </si>
   <si>
+    <t>nbAdjacence</t>
+  </si>
+  <si>
     <t>conditionFeedbackAdjacence</t>
   </si>
   <si>
-    <t>feedbackAdjacence</t>
+    <t>feedbackAdjacenceAttractivité</t>
   </si>
   <si>
     <t>conditionRessources</t>
@@ -167,12 +170,6 @@
   </si>
   <si>
     <t>V9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bar </t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>coutTouriste</t>
@@ -690,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -707,8 +704,8 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -720,6 +717,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -1024,7 +1024,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:X74"/>
+  <dimension ref="A1:Y74"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
@@ -1051,11 +1051,12 @@
     <col min="17" max="17" style="8" width="11.290714285714287" customWidth="1" bestFit="1"/>
     <col min="18" max="18" style="8" width="11.290714285714287" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="10" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="10" width="25.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="10" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="10" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="10" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="10" width="29.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="10" width="25.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="11" width="28.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="10" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="10" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="10" width="29.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1119,10 +1120,10 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
@@ -1131,19 +1132,22 @@
       <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" s="4">
         <v>2</v>
@@ -1168,24 +1172,25 @@
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
+      <c r="V2" s="6"/>
       <c r="W2" s="3"/>
-      <c r="X2" s="3" t="s">
-        <v>28</v>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E3" s="4">
         <v>1</v>
@@ -1208,24 +1213,25 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
+      <c r="V3" s="6"/>
       <c r="W3" s="3"/>
-      <c r="X3" s="3" t="s">
-        <v>31</v>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" s="4">
         <v>2</v>
@@ -1248,24 +1254,25 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
+      <c r="V4" s="6"/>
       <c r="W4" s="3"/>
-      <c r="X4" s="3" t="s">
-        <v>34</v>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="4">
         <v>3</v>
@@ -1288,24 +1295,25 @@
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
+      <c r="V5" s="6"/>
       <c r="W5" s="3"/>
-      <c r="X5" s="3" t="s">
-        <v>37</v>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="4">
         <v>1</v>
@@ -1328,24 +1336,25 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
+      <c r="V6" s="6"/>
       <c r="W6" s="3"/>
-      <c r="X6" s="3" t="s">
-        <v>40</v>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="4">
         <v>1</v>
@@ -1370,24 +1379,25 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
+      <c r="V7" s="6"/>
       <c r="W7" s="3"/>
-      <c r="X7" s="3" t="s">
-        <v>43</v>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4">
         <v>3</v>
@@ -1410,24 +1420,25 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
+      <c r="V8" s="6"/>
       <c r="W8" s="3"/>
-      <c r="X8" s="3" t="s">
-        <v>46</v>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E9" s="4">
         <v>3</v>
@@ -1450,24 +1461,25 @@
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
+      <c r="V9" s="6"/>
       <c r="W9" s="3"/>
-      <c r="X9" s="3" t="s">
-        <v>49</v>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" s="4">
         <v>2</v>
@@ -1487,33 +1499,32 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
-      <c r="S10" s="6" t="s">
+      <c r="S10" s="1"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="T10" s="3" t="s">
+      <c r="V10" s="2">
+        <v>1</v>
+      </c>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="U10" s="2">
-        <v>1</v>
-      </c>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E11" s="4">
         <v>1</v>
@@ -1536,24 +1547,25 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
+      <c r="V11" s="6"/>
       <c r="W11" s="3"/>
-      <c r="X11" s="3" t="s">
-        <v>57</v>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
@@ -1576,24 +1588,25 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
+      <c r="V12" s="6"/>
       <c r="W12" s="3"/>
-      <c r="X12" s="3" t="s">
-        <v>60</v>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E13" s="4">
         <v>3</v>
@@ -1616,24 +1629,25 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
+      <c r="V13" s="6"/>
       <c r="W13" s="3"/>
-      <c r="X13" s="3" t="s">
-        <v>63</v>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="E14" s="4">
         <v>1</v>
@@ -1656,22 +1670,23 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
+      <c r="V14" s="6"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E15" s="4">
         <v>3</v>
@@ -1700,22 +1715,23 @@
       </c>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
+      <c r="V15" s="6"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="C16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E16" s="4">
         <v>3</v>
@@ -1738,22 +1754,23 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
+      <c r="V16" s="6"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="C17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E17" s="4">
         <v>1</v>
@@ -1774,22 +1791,23 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
+      <c r="V17" s="6"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="C18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E18" s="4">
         <v>2</v>
@@ -1810,22 +1828,23 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
+      <c r="V18" s="6"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="C19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E19" s="4">
         <v>2</v>
@@ -1848,22 +1867,23 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
+      <c r="V19" s="6"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="C20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E20" s="4">
         <v>2</v>
@@ -1886,22 +1906,23 @@
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
+      <c r="V20" s="6"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="C21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E21" s="4">
         <v>1</v>
@@ -1922,22 +1943,23 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
+      <c r="V21" s="6"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="C22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E22" s="4">
         <v>1</v>
@@ -1958,22 +1980,23 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
+      <c r="V22" s="6"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="C23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E23" s="4">
         <v>3</v>
@@ -1996,22 +2019,23 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
+      <c r="V23" s="6"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="C24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E24" s="4">
         <v>3</v>
@@ -2034,22 +2058,23 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
-      <c r="V24" s="3"/>
+      <c r="V24" s="6"/>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="C25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E25" s="4">
         <v>1</v>
@@ -2072,22 +2097,23 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
+      <c r="V25" s="6"/>
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="C26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E26" s="4">
         <v>1</v>
@@ -2114,22 +2140,23 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
+      <c r="V26" s="6"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="C27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E27" s="4">
         <v>1</v>
@@ -2152,22 +2179,23 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
-      <c r="V27" s="3"/>
+      <c r="V27" s="6"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="E28" s="4">
         <v>3</v>
@@ -2190,22 +2218,23 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
-      <c r="V28" s="3"/>
+      <c r="V28" s="6"/>
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+      <c r="Y28" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="E29" s="4">
         <v>2</v>
@@ -2228,22 +2257,23 @@
       </c>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
+      <c r="V29" s="6"/>
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+      <c r="Y29" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E30" s="4">
         <v>2</v>
@@ -2266,26 +2296,27 @@
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
       <c r="U30" s="3"/>
-      <c r="V30" s="1" t="s">
+      <c r="V30" s="6"/>
+      <c r="W30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="X30" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="W30" s="1" t="s">
+      <c r="Y30" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+      <c r="A31" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="X30" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="C31" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E31" s="4">
         <v>3</v>
@@ -2306,26 +2337,27 @@
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
       <c r="S31" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
-      <c r="V31" s="3"/>
+      <c r="V31" s="6"/>
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+      <c r="Y31" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="C32" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E32" s="4">
         <v>3</v>
@@ -2348,22 +2380,23 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
-      <c r="V32" s="3"/>
+      <c r="V32" s="6"/>
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+      <c r="Y32" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="C33" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E33" s="4">
         <v>2</v>
@@ -2386,22 +2419,23 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
-      <c r="V33" s="3"/>
+      <c r="V33" s="6"/>
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+      <c r="Y33" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="C34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E34" s="4">
         <v>1</v>
@@ -2422,22 +2456,23 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
-      <c r="V34" s="3"/>
+      <c r="V34" s="6"/>
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+      <c r="Y34" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="C35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E35" s="4">
         <v>2</v>
@@ -2460,22 +2495,23 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
       <c r="U35" s="3"/>
-      <c r="V35" s="3"/>
+      <c r="V35" s="6"/>
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+      <c r="Y35" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="C36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E36" s="4">
         <v>3</v>
@@ -2496,22 +2532,23 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
-      <c r="V36" s="3"/>
+      <c r="V36" s="6"/>
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+      <c r="Y36" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="C37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E37" s="4">
         <v>3</v>
@@ -2534,22 +2571,23 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
       <c r="U37" s="3"/>
-      <c r="V37" s="3"/>
+      <c r="V37" s="6"/>
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+      <c r="Y37" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="C38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E38" s="4">
         <v>3</v>
@@ -2574,26 +2612,29 @@
       </c>
       <c r="R38" s="5"/>
       <c r="S38" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="T38" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="T38" s="6">
+        <v>2</v>
+      </c>
       <c r="U38" s="3"/>
-      <c r="V38" s="3"/>
+      <c r="V38" s="6"/>
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+      <c r="Y38" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="C39" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E39" s="4">
         <v>2</v>
@@ -2616,22 +2657,23 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
       <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
+      <c r="V39" s="6"/>
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+      <c r="Y39" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="C40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E40" s="4">
         <v>2</v>
@@ -2652,22 +2694,23 @@
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
-      <c r="V40" s="3"/>
+      <c r="V40" s="6"/>
       <c r="W40" s="3"/>
       <c r="X40" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+      <c r="Y40" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="E41" s="4">
         <v>2</v>
@@ -2688,22 +2731,23 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
       <c r="U41" s="3"/>
-      <c r="V41" s="3"/>
+      <c r="V41" s="6"/>
       <c r="W41" s="3"/>
       <c r="X41" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+      <c r="Y41" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="E42" s="4">
         <v>1</v>
@@ -2726,22 +2770,23 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
       <c r="U42" s="3"/>
-      <c r="V42" s="3"/>
+      <c r="V42" s="6"/>
       <c r="W42" s="3"/>
       <c r="X42" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+      <c r="Y42" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="E43" s="4">
         <v>2</v>
@@ -2762,22 +2807,23 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
       <c r="U43" s="3"/>
-      <c r="V43" s="3"/>
+      <c r="V43" s="6"/>
       <c r="W43" s="3"/>
       <c r="X43" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+      <c r="Y43" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="C44" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E44" s="4">
         <v>2</v>
@@ -2798,26 +2844,27 @@
       <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
       <c r="S44" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T44" s="3"/>
       <c r="U44" s="3"/>
-      <c r="V44" s="3"/>
+      <c r="V44" s="6"/>
       <c r="W44" s="3"/>
       <c r="X44" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+      <c r="Y44" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="E45" s="4">
         <v>1</v>
@@ -2838,22 +2885,23 @@
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
       <c r="U45" s="3"/>
-      <c r="V45" s="3"/>
+      <c r="V45" s="6"/>
       <c r="W45" s="3"/>
       <c r="X45" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+      <c r="Y45" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="C46" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E46" s="4">
         <v>2</v>
@@ -2872,26 +2920,27 @@
       <c r="Q46" s="5"/>
       <c r="R46" s="5"/>
       <c r="S46" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T46" s="3"/>
       <c r="U46" s="3"/>
-      <c r="V46" s="3"/>
+      <c r="V46" s="6"/>
       <c r="W46" s="3"/>
       <c r="X46" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+      <c r="Y46" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="C47" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E47" s="4">
         <v>2</v>
@@ -2912,22 +2961,23 @@
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
       <c r="U47" s="3"/>
-      <c r="V47" s="3"/>
+      <c r="V47" s="6"/>
       <c r="W47" s="3"/>
       <c r="X47" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+      <c r="Y47" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="C48" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E48" s="4">
         <v>3</v>
@@ -2950,22 +3000,23 @@
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
-      <c r="V48" s="3"/>
+      <c r="V48" s="6"/>
       <c r="W48" s="3"/>
       <c r="X48" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+      <c r="Y48" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="C49" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E49" s="4">
         <v>3</v>
@@ -2986,22 +3037,23 @@
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
       <c r="U49" s="3"/>
-      <c r="V49" s="3"/>
+      <c r="V49" s="6"/>
       <c r="W49" s="3"/>
       <c r="X49" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+      <c r="Y49" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="C50" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E50" s="4">
         <v>2</v>
@@ -3024,22 +3076,23 @@
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
       <c r="U50" s="3"/>
-      <c r="V50" s="3"/>
+      <c r="V50" s="6"/>
       <c r="W50" s="3"/>
       <c r="X50" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+      <c r="Y50" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="C51" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E51" s="4">
         <v>2</v>
@@ -3062,22 +3115,23 @@
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
       <c r="U51" s="3"/>
-      <c r="V51" s="3"/>
+      <c r="V51" s="6"/>
       <c r="W51" s="3"/>
       <c r="X51" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+      <c r="Y51" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="C52" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E52" s="4">
         <v>2</v>
@@ -3098,22 +3152,23 @@
       <c r="S52" s="3"/>
       <c r="T52" s="3"/>
       <c r="U52" s="3"/>
-      <c r="V52" s="3"/>
+      <c r="V52" s="6"/>
       <c r="W52" s="3"/>
       <c r="X52" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+      <c r="Y52" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="C53" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E53" s="4">
         <v>3</v>
@@ -3134,22 +3189,23 @@
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
       <c r="U53" s="3"/>
-      <c r="V53" s="3"/>
+      <c r="V53" s="6"/>
       <c r="W53" s="3"/>
       <c r="X53" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+      <c r="Y53" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="C54" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E54" s="4">
         <v>2</v>
@@ -3176,22 +3232,23 @@
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
       <c r="U54" s="3"/>
-      <c r="V54" s="3"/>
+      <c r="V54" s="6"/>
       <c r="W54" s="3"/>
       <c r="X54" s="3"/>
+      <c r="Y54" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="C55" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E55" s="4">
         <v>2</v>
@@ -3216,22 +3273,23 @@
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
       <c r="U55" s="3"/>
-      <c r="V55" s="3"/>
+      <c r="V55" s="6"/>
       <c r="W55" s="3"/>
       <c r="X55" s="3"/>
+      <c r="Y55" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="C56" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="E56" s="4">
         <v>3</v>
@@ -3256,26 +3314,27 @@
       <c r="Q56" s="5"/>
       <c r="R56" s="5"/>
       <c r="S56" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T56" s="3"/>
       <c r="U56" s="3"/>
-      <c r="V56" s="3"/>
+      <c r="V56" s="6"/>
       <c r="W56" s="3"/>
       <c r="X56" s="3"/>
+      <c r="Y56" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="C57" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E57" s="4">
         <v>2</v>
@@ -3294,26 +3353,27 @@
       <c r="Q57" s="5"/>
       <c r="R57" s="5"/>
       <c r="S57" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T57" s="3"/>
       <c r="U57" s="3"/>
-      <c r="V57" s="3"/>
+      <c r="V57" s="6"/>
       <c r="W57" s="3"/>
       <c r="X57" s="3"/>
+      <c r="Y57" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="C58" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E58" s="4">
         <v>3</v>
@@ -3336,22 +3396,23 @@
       <c r="S58" s="3"/>
       <c r="T58" s="3"/>
       <c r="U58" s="3"/>
-      <c r="V58" s="3"/>
+      <c r="V58" s="6"/>
       <c r="W58" s="3"/>
       <c r="X58" s="3"/>
+      <c r="Y58" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="E59" s="4">
         <v>1</v>
@@ -3374,22 +3435,23 @@
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
       <c r="U59" s="3"/>
-      <c r="V59" s="3"/>
+      <c r="V59" s="6"/>
       <c r="W59" s="3"/>
       <c r="X59" s="3"/>
+      <c r="Y59" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="E60" s="4">
         <v>3</v>
@@ -3412,22 +3474,23 @@
       <c r="S60" s="3"/>
       <c r="T60" s="3"/>
       <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
+      <c r="V60" s="6"/>
       <c r="W60" s="3"/>
       <c r="X60" s="3"/>
+      <c r="Y60" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="C61" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E61" s="4">
         <v>1</v>
@@ -3450,22 +3513,23 @@
       <c r="S61" s="3"/>
       <c r="T61" s="3"/>
       <c r="U61" s="3"/>
-      <c r="V61" s="3"/>
+      <c r="V61" s="6"/>
       <c r="W61" s="3"/>
       <c r="X61" s="3"/>
+      <c r="Y61" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="C62" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E62" s="4">
         <v>3</v>
@@ -3488,22 +3552,23 @@
       <c r="S62" s="3"/>
       <c r="T62" s="3"/>
       <c r="U62" s="3"/>
-      <c r="V62" s="3"/>
+      <c r="V62" s="6"/>
       <c r="W62" s="3"/>
       <c r="X62" s="3"/>
+      <c r="Y62" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="C63" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E63" s="4">
         <v>1</v>
@@ -3524,26 +3589,27 @@
       <c r="Q63" s="5"/>
       <c r="R63" s="5"/>
       <c r="S63" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T63" s="3"/>
       <c r="U63" s="3"/>
-      <c r="V63" s="3"/>
+      <c r="V63" s="6"/>
       <c r="W63" s="3"/>
       <c r="X63" s="3"/>
+      <c r="Y63" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="C64" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E64" s="4">
         <v>2</v>
@@ -3566,22 +3632,23 @@
       <c r="S64" s="3"/>
       <c r="T64" s="3"/>
       <c r="U64" s="3"/>
-      <c r="V64" s="3"/>
+      <c r="V64" s="6"/>
       <c r="W64" s="3"/>
       <c r="X64" s="3"/>
+      <c r="Y64" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="C65" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E65" s="4">
         <v>2</v>
@@ -3602,26 +3669,27 @@
       <c r="Q65" s="5"/>
       <c r="R65" s="5"/>
       <c r="S65" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T65" s="3"/>
       <c r="U65" s="3"/>
-      <c r="V65" s="3"/>
+      <c r="V65" s="6"/>
       <c r="W65" s="3"/>
       <c r="X65" s="3"/>
+      <c r="Y65" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="C66" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E66" s="4">
         <v>4</v>
@@ -3646,22 +3714,23 @@
       <c r="S66" s="3"/>
       <c r="T66" s="3"/>
       <c r="U66" s="3"/>
-      <c r="V66" s="3"/>
+      <c r="V66" s="6"/>
       <c r="W66" s="3"/>
       <c r="X66" s="3"/>
+      <c r="Y66" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="C67" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E67" s="4">
         <v>3</v>
@@ -3690,22 +3759,23 @@
       </c>
       <c r="T67" s="3"/>
       <c r="U67" s="3"/>
-      <c r="V67" s="3"/>
+      <c r="V67" s="6"/>
       <c r="W67" s="3"/>
       <c r="X67" s="3"/>
+      <c r="Y67" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="C68" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E68" s="4">
         <v>1</v>
@@ -3730,22 +3800,23 @@
       <c r="S68" s="3"/>
       <c r="T68" s="3"/>
       <c r="U68" s="3"/>
-      <c r="V68" s="3"/>
+      <c r="V68" s="6"/>
       <c r="W68" s="3"/>
       <c r="X68" s="3"/>
+      <c r="Y68" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="C69" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E69" s="4">
         <v>2</v>
@@ -3766,26 +3837,27 @@
       <c r="Q69" s="5"/>
       <c r="R69" s="5"/>
       <c r="S69" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T69" s="3"/>
       <c r="U69" s="3"/>
-      <c r="V69" s="3"/>
+      <c r="V69" s="6"/>
       <c r="W69" s="3"/>
       <c r="X69" s="3"/>
+      <c r="Y69" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="C70" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E70" s="4">
         <v>2</v>
@@ -3806,26 +3878,27 @@
       <c r="Q70" s="5"/>
       <c r="R70" s="5"/>
       <c r="S70" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T70" s="3"/>
       <c r="U70" s="3"/>
-      <c r="V70" s="3"/>
+      <c r="V70" s="6"/>
       <c r="W70" s="3"/>
       <c r="X70" s="3"/>
+      <c r="Y70" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="C71" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E71" s="4">
         <v>3</v>
@@ -3848,22 +3921,23 @@
       <c r="S71" s="3"/>
       <c r="T71" s="3"/>
       <c r="U71" s="3"/>
-      <c r="V71" s="3"/>
+      <c r="V71" s="6"/>
       <c r="W71" s="3"/>
       <c r="X71" s="3"/>
+      <c r="Y71" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="C72" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E72" s="4">
         <v>2</v>
@@ -3882,26 +3956,27 @@
       <c r="Q72" s="5"/>
       <c r="R72" s="5"/>
       <c r="S72" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="T72" s="3"/>
       <c r="U72" s="3"/>
-      <c r="V72" s="3"/>
+      <c r="V72" s="6"/>
       <c r="W72" s="3"/>
       <c r="X72" s="3"/>
+      <c r="Y72" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="E73" s="4">
         <v>1</v>
@@ -3924,22 +3999,23 @@
       <c r="S73" s="3"/>
       <c r="T73" s="3"/>
       <c r="U73" s="3"/>
-      <c r="V73" s="3"/>
+      <c r="V73" s="6"/>
       <c r="W73" s="3"/>
       <c r="X73" s="3"/>
+      <c r="Y73" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="C74" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="E74" s="4">
         <v>2</v>
@@ -3960,13 +4036,14 @@
       <c r="Q74" s="5"/>
       <c r="R74" s="5"/>
       <c r="S74" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T74" s="3"/>
       <c r="U74" s="3"/>
-      <c r="V74" s="3"/>
+      <c r="V74" s="6"/>
       <c r="W74" s="3"/>
       <c r="X74" s="3"/>
+      <c r="Y74" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ajout d'un name aux actions + correction bugs
</commit_message>
<xml_diff>
--- a/data/solutre_hex_inst.xlsx
+++ b/data/solutre_hex_inst.xlsx
@@ -639,7 +639,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,6 +656,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -687,13 +693,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -704,8 +713,8 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1032,31 +1041,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="45.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="8" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="8" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="8" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="8" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="8" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="10" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="10" width="25.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="11" width="28.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="10" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="10" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="10" width="29.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="45.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="9" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="9" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="9" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="9" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="11" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="11" width="25.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="12" width="28.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="11" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="11" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="11" width="29.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1120,7 +1129,7 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="2" t="s">
@@ -1149,33 +1158,33 @@
       <c r="D2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>2</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="4">
-        <v>1</v>
-      </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="4">
-        <v>1</v>
-      </c>
-      <c r="S2" s="3"/>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="5">
+        <v>1</v>
+      </c>
+      <c r="S2" s="4"/>
       <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3" t="s">
+      <c r="U2" s="4"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1192,31 +1201,31 @@
       <c r="D3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="4">
+      <c r="G3" s="5">
         <v>1</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="3"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="4"/>
       <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3" t="s">
+      <c r="U3" s="4"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1233,31 +1242,31 @@
       <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="5">
         <v>2</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="3"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="5">
+        <v>1</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="4"/>
       <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3" t="s">
+      <c r="U4" s="4"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1274,31 +1283,31 @@
       <c r="D5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <v>3</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="4">
-        <v>1</v>
-      </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="3"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="5">
+        <v>1</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="4"/>
       <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3" t="s">
+      <c r="U5" s="4"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1315,31 +1324,31 @@
       <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="5">
         <v>1</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="4">
-        <v>1</v>
-      </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="3"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="5">
+        <v>1</v>
+      </c>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="4"/>
       <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3" t="s">
+      <c r="U6" s="4"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1356,33 +1365,33 @@
       <c r="D7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="5">
         <v>1</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="4">
+      <c r="G7" s="5">
         <v>-1</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="4">
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="5">
         <v>0</v>
       </c>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="3"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="4"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3" t="s">
+      <c r="U7" s="4"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1399,31 +1408,31 @@
       <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="5">
         <v>3</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="4">
-        <v>1</v>
-      </c>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="3"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="5">
+        <v>1</v>
+      </c>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="4"/>
       <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3" t="s">
+      <c r="U8" s="4"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1440,31 +1449,31 @@
       <c r="D9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="5">
         <v>3</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="4">
-        <v>1</v>
-      </c>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="3"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="5">
+        <v>1</v>
+      </c>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="4"/>
       <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3" t="s">
+      <c r="U9" s="4"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1481,35 +1490,35 @@
       <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="5">
         <v>2</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="4">
-        <v>1</v>
-      </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="5">
+        <v>1</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
       <c r="S10" s="1"/>
       <c r="T10" s="3"/>
-      <c r="U10" s="3" t="s">
+      <c r="U10" s="4" t="s">
         <v>52</v>
       </c>
       <c r="V10" s="2">
         <v>1</v>
       </c>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3" t="s">
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1526,31 +1535,31 @@
       <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="5">
         <v>1</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="4">
-        <v>1</v>
-      </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="3"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="5">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="4"/>
       <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3" t="s">
+      <c r="U11" s="4"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1567,31 +1576,31 @@
       <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="5">
         <v>1</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="4">
-        <v>1</v>
-      </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="3"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="5">
+        <v>1</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="4"/>
       <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
-      <c r="Y12" s="3" t="s">
+      <c r="U12" s="4"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1608,31 +1617,31 @@
       <c r="D13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="5">
         <v>3</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="4">
-        <v>1</v>
-      </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="3"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="5">
+        <v>1</v>
+      </c>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="4"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3" t="s">
+      <c r="U13" s="4"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1649,31 +1658,31 @@
       <c r="D14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="5">
         <v>1</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="4">
-        <v>1</v>
-      </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="3"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="5">
+        <v>1</v>
+      </c>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="4"/>
       <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
@@ -1688,37 +1697,37 @@
       <c r="D15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="5">
         <v>3</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="4">
+      <c r="G15" s="5">
         <v>1</v>
       </c>
       <c r="H15" s="2"/>
-      <c r="I15" s="4">
-        <v>1</v>
-      </c>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="4">
-        <v>1</v>
-      </c>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="3" t="s">
+      <c r="I15" s="5">
+        <v>1</v>
+      </c>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="5">
+        <v>1</v>
+      </c>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="6"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
-      <c r="Y15" s="3"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
@@ -1733,31 +1742,31 @@
       <c r="D16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="5">
         <v>3</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="3"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="4"/>
       <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="6"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
@@ -1772,29 +1781,29 @@
       <c r="D17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="5">
         <v>1</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="3"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="4"/>
       <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="6"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
@@ -1809,29 +1818,29 @@
       <c r="D18" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="5">
         <v>2</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="3"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="4"/>
       <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
@@ -1846,31 +1855,31 @@
       <c r="D19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="5">
         <v>2</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="4">
-        <v>1</v>
-      </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="3"/>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="4"/>
       <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
@@ -1885,31 +1894,31 @@
       <c r="D20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="5">
         <v>2</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="4">
+      <c r="G20" s="5">
         <v>1</v>
       </c>
       <c r="H20" s="2"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="3"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="4"/>
       <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
@@ -1924,29 +1933,29 @@
       <c r="D21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="5">
         <v>1</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="3"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="4"/>
       <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="6"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
@@ -1961,29 +1970,29 @@
       <c r="D22" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="5">
         <v>1</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="3"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="4"/>
       <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="6"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
@@ -1998,31 +2007,31 @@
       <c r="D23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="5">
         <v>3</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="4">
-        <v>1</v>
-      </c>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="3"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="5">
+        <v>1</v>
+      </c>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="4"/>
       <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
@@ -2037,31 +2046,31 @@
       <c r="D24" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="5">
         <v>3</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="4">
-        <v>1</v>
-      </c>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="3"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="5">
+        <v>1</v>
+      </c>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="4"/>
       <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-      <c r="V24" s="6"/>
-      <c r="W24" s="3"/>
-      <c r="X24" s="3"/>
-      <c r="Y24" s="3"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1" t="s">
@@ -2076,31 +2085,31 @@
       <c r="D25" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="5">
         <v>1</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="4">
-        <v>1</v>
-      </c>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="3"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="5">
+        <v>1</v>
+      </c>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="4"/>
       <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="6"/>
-      <c r="W25" s="3"/>
-      <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
@@ -2115,35 +2124,35 @@
       <c r="D26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E26" s="4">
-        <v>1</v>
-      </c>
-      <c r="F26" s="4">
+      <c r="E26" s="5">
+        <v>1</v>
+      </c>
+      <c r="F26" s="5">
         <v>-1</v>
       </c>
       <c r="G26" s="2"/>
-      <c r="H26" s="4">
+      <c r="H26" s="5">
         <v>-1</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26" s="5">
         <v>6</v>
       </c>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="3"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="4"/>
       <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-      <c r="V26" s="6"/>
-      <c r="W26" s="3"/>
-      <c r="X26" s="3"/>
-      <c r="Y26" s="3"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1" t="s">
@@ -2158,31 +2167,31 @@
       <c r="D27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="5">
         <v>1</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="4">
-        <v>1</v>
-      </c>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="3"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="5">
+        <v>1</v>
+      </c>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="4"/>
       <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
-      <c r="V27" s="6"/>
-      <c r="W27" s="3"/>
-      <c r="X27" s="3"/>
-      <c r="Y27" s="3"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
@@ -2197,31 +2206,31 @@
       <c r="D28" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="5">
         <v>3</v>
       </c>
       <c r="F28" s="2"/>
-      <c r="G28" s="4">
+      <c r="G28" s="5">
         <v>1</v>
       </c>
       <c r="H28" s="2"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="3"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="4"/>
       <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
-      <c r="V28" s="6"/>
-      <c r="W28" s="3"/>
-      <c r="X28" s="3"/>
-      <c r="Y28" s="3"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1" t="s">
@@ -2236,31 +2245,31 @@
       <c r="D29" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="5">
         <v>2</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="3" t="s">
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="4" t="s">
         <v>14</v>
       </c>
       <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
-      <c r="V29" s="6"/>
-      <c r="W29" s="3"/>
-      <c r="X29" s="3"/>
-      <c r="Y29" s="3"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1" t="s">
@@ -2275,35 +2284,35 @@
       <c r="D30" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="5">
         <v>2</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="4">
-        <v>1</v>
-      </c>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="3"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="5">
+        <v>1</v>
+      </c>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="4"/>
       <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-      <c r="V30" s="6"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="7"/>
       <c r="W30" s="1" t="s">
         <v>104</v>
       </c>
       <c r="X30" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="Y30" s="3"/>
+      <c r="Y30" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="1" t="s">
@@ -2318,33 +2327,33 @@
       <c r="D31" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="5">
         <v>3</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="4">
-        <v>1</v>
-      </c>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="3" t="s">
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="5">
+        <v>1</v>
+      </c>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="4" t="s">
         <v>108</v>
       </c>
       <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
-      <c r="V31" s="6"/>
-      <c r="W31" s="3"/>
-      <c r="X31" s="3"/>
-      <c r="Y31" s="3"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="1" t="s">
@@ -2359,31 +2368,31 @@
       <c r="D32" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="5">
         <v>3</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="4">
-        <v>1</v>
-      </c>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="3"/>
+      <c r="H32" s="5">
+        <v>1</v>
+      </c>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="4"/>
       <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
-      <c r="V32" s="6"/>
-      <c r="W32" s="3"/>
-      <c r="X32" s="3"/>
-      <c r="Y32" s="3"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="4"/>
+      <c r="X32" s="4"/>
+      <c r="Y32" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="1" t="s">
@@ -2398,31 +2407,31 @@
       <c r="D33" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="5">
         <v>2</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="4">
-        <v>1</v>
-      </c>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="3"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="5">
+        <v>1</v>
+      </c>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="4"/>
       <c r="T33" s="3"/>
-      <c r="U33" s="3"/>
-      <c r="V33" s="6"/>
-      <c r="W33" s="3"/>
-      <c r="X33" s="3"/>
-      <c r="Y33" s="3"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="1" t="s">
@@ -2437,29 +2446,29 @@
       <c r="D34" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="5">
         <v>1</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="3"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="4"/>
       <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="3"/>
-      <c r="X34" s="3"/>
-      <c r="Y34" s="3"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="1" t="s">
@@ -2474,31 +2483,31 @@
       <c r="D35" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="5">
         <v>2</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="4">
-        <v>1</v>
-      </c>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="5"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
-      <c r="R35" s="5"/>
-      <c r="S35" s="3"/>
+      <c r="H35" s="5">
+        <v>1</v>
+      </c>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="4"/>
       <c r="T35" s="3"/>
-      <c r="U35" s="3"/>
-      <c r="V35" s="6"/>
-      <c r="W35" s="3"/>
-      <c r="X35" s="3"/>
-      <c r="Y35" s="3"/>
+      <c r="U35" s="4"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="4"/>
+      <c r="X35" s="4"/>
+      <c r="Y35" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="1" t="s">
@@ -2513,29 +2522,29 @@
       <c r="D36" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="5">
         <v>3</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="3"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="4"/>
       <c r="T36" s="3"/>
-      <c r="U36" s="3"/>
-      <c r="V36" s="6"/>
-      <c r="W36" s="3"/>
-      <c r="X36" s="3"/>
-      <c r="Y36" s="3"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="1" t="s">
@@ -2550,31 +2559,31 @@
       <c r="D37" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="5">
         <v>3</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="5">
         <v>1</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="3"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="4"/>
       <c r="T37" s="3"/>
-      <c r="U37" s="3"/>
-      <c r="V37" s="6"/>
-      <c r="W37" s="3"/>
-      <c r="X37" s="3"/>
-      <c r="Y37" s="3"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="7"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="1" t="s">
@@ -2589,39 +2598,39 @@
       <c r="D38" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="5">
         <v>3</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="5">
         <v>1</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="4">
-        <v>1</v>
-      </c>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="4">
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="5">
+        <v>1</v>
+      </c>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="5">
         <v>2</v>
       </c>
-      <c r="R38" s="5"/>
-      <c r="S38" s="3" t="s">
+      <c r="R38" s="6"/>
+      <c r="S38" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="T38" s="6">
+      <c r="T38" s="7">
         <v>2</v>
       </c>
-      <c r="U38" s="3"/>
-      <c r="V38" s="6"/>
-      <c r="W38" s="3"/>
-      <c r="X38" s="3"/>
-      <c r="Y38" s="3"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="4"/>
+      <c r="X38" s="4"/>
+      <c r="Y38" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="1" t="s">
@@ -2636,31 +2645,31 @@
       <c r="D39" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="5">
         <v>2</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="4">
-        <v>1</v>
-      </c>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="3"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="5">
+        <v>1</v>
+      </c>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="4"/>
       <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="6"/>
-      <c r="W39" s="3"/>
-      <c r="X39" s="3"/>
-      <c r="Y39" s="3"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="7"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="1" t="s">
@@ -2675,29 +2684,29 @@
       <c r="D40" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="5">
         <v>2</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="3"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="4"/>
       <c r="T40" s="3"/>
-      <c r="U40" s="3"/>
-      <c r="V40" s="6"/>
-      <c r="W40" s="3"/>
-      <c r="X40" s="3"/>
-      <c r="Y40" s="3"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="7"/>
+      <c r="W40" s="4"/>
+      <c r="X40" s="4"/>
+      <c r="Y40" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="1" t="s">
@@ -2712,29 +2721,29 @@
       <c r="D41" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="5">
         <v>2</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="3"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="4"/>
       <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
-      <c r="V41" s="6"/>
-      <c r="W41" s="3"/>
-      <c r="X41" s="3"/>
-      <c r="Y41" s="3"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="7"/>
+      <c r="W41" s="4"/>
+      <c r="X41" s="4"/>
+      <c r="Y41" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="1" t="s">
@@ -2749,31 +2758,31 @@
       <c r="D42" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E42" s="4">
-        <v>1</v>
-      </c>
-      <c r="F42" s="4">
+      <c r="E42" s="5">
+        <v>1</v>
+      </c>
+      <c r="F42" s="5">
         <v>-1</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="3"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="4"/>
       <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
-      <c r="V42" s="6"/>
-      <c r="W42" s="3"/>
-      <c r="X42" s="3"/>
-      <c r="Y42" s="3"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="7"/>
+      <c r="W42" s="4"/>
+      <c r="X42" s="4"/>
+      <c r="Y42" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="1" t="s">
@@ -2788,29 +2797,29 @@
       <c r="D43" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="5">
         <v>2</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="5"/>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="3"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="6"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="4"/>
       <c r="T43" s="3"/>
-      <c r="U43" s="3"/>
-      <c r="V43" s="6"/>
-      <c r="W43" s="3"/>
-      <c r="X43" s="3"/>
-      <c r="Y43" s="3"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="7"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="4"/>
+      <c r="Y43" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="1" t="s">
@@ -2825,33 +2834,33 @@
       <c r="D44" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="5">
         <v>2</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
-      <c r="I44" s="4">
-        <v>1</v>
-      </c>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="5"/>
-      <c r="R44" s="5"/>
-      <c r="S44" s="3" t="s">
+      <c r="I44" s="5">
+        <v>1</v>
+      </c>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
+      <c r="P44" s="6"/>
+      <c r="Q44" s="6"/>
+      <c r="R44" s="6"/>
+      <c r="S44" s="4" t="s">
         <v>123</v>
       </c>
       <c r="T44" s="3"/>
-      <c r="U44" s="3"/>
-      <c r="V44" s="6"/>
-      <c r="W44" s="3"/>
-      <c r="X44" s="3"/>
-      <c r="Y44" s="3"/>
+      <c r="U44" s="4"/>
+      <c r="V44" s="7"/>
+      <c r="W44" s="4"/>
+      <c r="X44" s="4"/>
+      <c r="Y44" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="1" t="s">
@@ -2866,29 +2875,29 @@
       <c r="D45" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="5">
         <v>1</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="3"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="4"/>
       <c r="T45" s="3"/>
-      <c r="U45" s="3"/>
-      <c r="V45" s="6"/>
-      <c r="W45" s="3"/>
-      <c r="X45" s="3"/>
-      <c r="Y45" s="3"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="7"/>
+      <c r="W45" s="4"/>
+      <c r="X45" s="4"/>
+      <c r="Y45" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="1" t="s">
@@ -2903,31 +2912,31 @@
       <c r="D46" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46" s="5">
         <v>2</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="5"/>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="3" t="s">
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="6"/>
+      <c r="P46" s="6"/>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6"/>
+      <c r="S46" s="4" t="s">
         <v>68</v>
       </c>
       <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
-      <c r="V46" s="6"/>
-      <c r="W46" s="3"/>
-      <c r="X46" s="3"/>
-      <c r="Y46" s="3"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="7"/>
+      <c r="W46" s="4"/>
+      <c r="X46" s="4"/>
+      <c r="Y46" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="1" t="s">
@@ -2942,29 +2951,29 @@
       <c r="D47" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E47" s="4">
+      <c r="E47" s="5">
         <v>2</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5"/>
-      <c r="S47" s="3"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="6"/>
+      <c r="P47" s="6"/>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6"/>
+      <c r="S47" s="4"/>
       <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
-      <c r="V47" s="6"/>
-      <c r="W47" s="3"/>
-      <c r="X47" s="3"/>
-      <c r="Y47" s="3"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="7"/>
+      <c r="W47" s="4"/>
+      <c r="X47" s="4"/>
+      <c r="Y47" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="1" t="s">
@@ -2979,31 +2988,31 @@
       <c r="D48" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E48" s="4">
+      <c r="E48" s="5">
         <v>3</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5"/>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5"/>
-      <c r="O48" s="4">
-        <v>1</v>
-      </c>
-      <c r="P48" s="5"/>
-      <c r="Q48" s="5"/>
-      <c r="R48" s="5"/>
-      <c r="S48" s="3"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+      <c r="N48" s="6"/>
+      <c r="O48" s="5">
+        <v>1</v>
+      </c>
+      <c r="P48" s="6"/>
+      <c r="Q48" s="6"/>
+      <c r="R48" s="6"/>
+      <c r="S48" s="4"/>
       <c r="T48" s="3"/>
-      <c r="U48" s="3"/>
-      <c r="V48" s="6"/>
-      <c r="W48" s="3"/>
-      <c r="X48" s="3"/>
-      <c r="Y48" s="3"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="7"/>
+      <c r="W48" s="4"/>
+      <c r="X48" s="4"/>
+      <c r="Y48" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="1" t="s">
@@ -3018,29 +3027,29 @@
       <c r="D49" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E49" s="4">
+      <c r="E49" s="5">
         <v>3</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="5"/>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="5"/>
-      <c r="R49" s="5"/>
-      <c r="S49" s="3"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
+      <c r="P49" s="6"/>
+      <c r="Q49" s="6"/>
+      <c r="R49" s="6"/>
+      <c r="S49" s="4"/>
       <c r="T49" s="3"/>
-      <c r="U49" s="3"/>
-      <c r="V49" s="6"/>
-      <c r="W49" s="3"/>
-      <c r="X49" s="3"/>
-      <c r="Y49" s="3"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="7"/>
+      <c r="W49" s="4"/>
+      <c r="X49" s="4"/>
+      <c r="Y49" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="1" t="s">
@@ -3055,31 +3064,31 @@
       <c r="D50" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E50" s="4">
+      <c r="E50" s="5">
         <v>2</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="4">
-        <v>1</v>
-      </c>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5"/>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="5"/>
-      <c r="R50" s="5"/>
-      <c r="S50" s="3"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="5">
+        <v>1</v>
+      </c>
+      <c r="N50" s="6"/>
+      <c r="O50" s="6"/>
+      <c r="P50" s="6"/>
+      <c r="Q50" s="6"/>
+      <c r="R50" s="6"/>
+      <c r="S50" s="4"/>
       <c r="T50" s="3"/>
-      <c r="U50" s="3"/>
-      <c r="V50" s="6"/>
-      <c r="W50" s="3"/>
-      <c r="X50" s="3"/>
-      <c r="Y50" s="3"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="7"/>
+      <c r="W50" s="4"/>
+      <c r="X50" s="4"/>
+      <c r="Y50" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="1" t="s">
@@ -3094,31 +3103,31 @@
       <c r="D51" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E51" s="4">
+      <c r="E51" s="5">
         <v>2</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="4">
-        <v>1</v>
-      </c>
-      <c r="P51" s="5"/>
-      <c r="Q51" s="5"/>
-      <c r="R51" s="5"/>
-      <c r="S51" s="3"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="5">
+        <v>1</v>
+      </c>
+      <c r="P51" s="6"/>
+      <c r="Q51" s="6"/>
+      <c r="R51" s="6"/>
+      <c r="S51" s="4"/>
       <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
-      <c r="V51" s="6"/>
-      <c r="W51" s="3"/>
-      <c r="X51" s="3"/>
-      <c r="Y51" s="3"/>
+      <c r="U51" s="4"/>
+      <c r="V51" s="7"/>
+      <c r="W51" s="4"/>
+      <c r="X51" s="4"/>
+      <c r="Y51" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="1" t="s">
@@ -3133,29 +3142,29 @@
       <c r="D52" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E52" s="4">
+      <c r="E52" s="5">
         <v>2</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="5"/>
-      <c r="R52" s="5"/>
-      <c r="S52" s="3"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+      <c r="P52" s="6"/>
+      <c r="Q52" s="6"/>
+      <c r="R52" s="6"/>
+      <c r="S52" s="4"/>
       <c r="T52" s="3"/>
-      <c r="U52" s="3"/>
-      <c r="V52" s="6"/>
-      <c r="W52" s="3"/>
-      <c r="X52" s="3"/>
-      <c r="Y52" s="3"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="7"/>
+      <c r="W52" s="4"/>
+      <c r="X52" s="4"/>
+      <c r="Y52" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="1" t="s">
@@ -3170,29 +3179,29 @@
       <c r="D53" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E53" s="4">
+      <c r="E53" s="5">
         <v>3</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
-      <c r="P53" s="5"/>
-      <c r="Q53" s="5"/>
-      <c r="R53" s="5"/>
-      <c r="S53" s="3"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+      <c r="P53" s="6"/>
+      <c r="Q53" s="6"/>
+      <c r="R53" s="6"/>
+      <c r="S53" s="4"/>
       <c r="T53" s="3"/>
-      <c r="U53" s="3"/>
-      <c r="V53" s="6"/>
-      <c r="W53" s="3"/>
-      <c r="X53" s="3"/>
-      <c r="Y53" s="3"/>
+      <c r="U53" s="4"/>
+      <c r="V53" s="7"/>
+      <c r="W53" s="4"/>
+      <c r="X53" s="4"/>
+      <c r="Y53" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="1" t="s">
@@ -3207,35 +3216,35 @@
       <c r="D54" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E54" s="4">
+      <c r="E54" s="5">
         <v>2</v>
       </c>
-      <c r="F54" s="4">
+      <c r="F54" s="5">
         <v>1</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="4">
-        <v>1</v>
-      </c>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5"/>
-      <c r="P54" s="5"/>
-      <c r="Q54" s="4">
-        <v>1</v>
-      </c>
-      <c r="R54" s="5"/>
-      <c r="S54" s="3"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="5">
+        <v>1</v>
+      </c>
+      <c r="M54" s="6"/>
+      <c r="N54" s="6"/>
+      <c r="O54" s="6"/>
+      <c r="P54" s="6"/>
+      <c r="Q54" s="5">
+        <v>1</v>
+      </c>
+      <c r="R54" s="6"/>
+      <c r="S54" s="4"/>
       <c r="T54" s="3"/>
-      <c r="U54" s="3"/>
-      <c r="V54" s="6"/>
-      <c r="W54" s="3"/>
-      <c r="X54" s="3"/>
-      <c r="Y54" s="3"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="7"/>
+      <c r="W54" s="4"/>
+      <c r="X54" s="4"/>
+      <c r="Y54" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="1" t="s">
@@ -3250,33 +3259,33 @@
       <c r="D55" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E55" s="4">
+      <c r="E55" s="5">
         <v>2</v>
       </c>
-      <c r="F55" s="4">
+      <c r="F55" s="5">
         <v>1</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
-      <c r="N55" s="4">
-        <v>1</v>
-      </c>
-      <c r="O55" s="5"/>
-      <c r="P55" s="5"/>
-      <c r="Q55" s="5"/>
-      <c r="R55" s="5"/>
-      <c r="S55" s="3"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+      <c r="M55" s="6"/>
+      <c r="N55" s="5">
+        <v>1</v>
+      </c>
+      <c r="O55" s="6"/>
+      <c r="P55" s="6"/>
+      <c r="Q55" s="6"/>
+      <c r="R55" s="6"/>
+      <c r="S55" s="4"/>
       <c r="T55" s="3"/>
-      <c r="U55" s="3"/>
-      <c r="V55" s="6"/>
-      <c r="W55" s="3"/>
-      <c r="X55" s="3"/>
-      <c r="Y55" s="3"/>
+      <c r="U55" s="4"/>
+      <c r="V55" s="7"/>
+      <c r="W55" s="4"/>
+      <c r="X55" s="4"/>
+      <c r="Y55" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="1" t="s">
@@ -3291,37 +3300,37 @@
       <c r="D56" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E56" s="4">
+      <c r="E56" s="5">
         <v>3</v>
       </c>
-      <c r="F56" s="4">
+      <c r="F56" s="5">
         <v>1</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
-      <c r="I56" s="4">
-        <v>1</v>
-      </c>
-      <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="4">
-        <v>1</v>
-      </c>
-      <c r="N56" s="5"/>
-      <c r="O56" s="5"/>
-      <c r="P56" s="5"/>
-      <c r="Q56" s="5"/>
-      <c r="R56" s="5"/>
-      <c r="S56" s="3" t="s">
+      <c r="I56" s="5">
+        <v>1</v>
+      </c>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="6"/>
+      <c r="M56" s="5">
+        <v>1</v>
+      </c>
+      <c r="N56" s="6"/>
+      <c r="O56" s="6"/>
+      <c r="P56" s="6"/>
+      <c r="Q56" s="6"/>
+      <c r="R56" s="6"/>
+      <c r="S56" s="4" t="s">
         <v>68</v>
       </c>
       <c r="T56" s="3"/>
-      <c r="U56" s="3"/>
-      <c r="V56" s="6"/>
-      <c r="W56" s="3"/>
-      <c r="X56" s="3"/>
-      <c r="Y56" s="3"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="7"/>
+      <c r="W56" s="4"/>
+      <c r="X56" s="4"/>
+      <c r="Y56" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="1" t="s">
@@ -3336,31 +3345,31 @@
       <c r="D57" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E57" s="4">
+      <c r="E57" s="5">
         <v>2</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
-      <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
-      <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
-      <c r="M57" s="5"/>
-      <c r="N57" s="5"/>
-      <c r="O57" s="5"/>
-      <c r="P57" s="5"/>
-      <c r="Q57" s="5"/>
-      <c r="R57" s="5"/>
-      <c r="S57" s="3" t="s">
+      <c r="I57" s="6"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="6"/>
+      <c r="L57" s="6"/>
+      <c r="M57" s="6"/>
+      <c r="N57" s="6"/>
+      <c r="O57" s="6"/>
+      <c r="P57" s="6"/>
+      <c r="Q57" s="6"/>
+      <c r="R57" s="6"/>
+      <c r="S57" s="4" t="s">
         <v>68</v>
       </c>
       <c r="T57" s="3"/>
-      <c r="U57" s="3"/>
-      <c r="V57" s="6"/>
-      <c r="W57" s="3"/>
-      <c r="X57" s="3"/>
-      <c r="Y57" s="3"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="7"/>
+      <c r="W57" s="4"/>
+      <c r="X57" s="4"/>
+      <c r="Y57" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="1" t="s">
@@ -3375,31 +3384,31 @@
       <c r="D58" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E58" s="4">
+      <c r="E58" s="5">
         <v>3</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
-      <c r="I58" s="5"/>
-      <c r="J58" s="5"/>
-      <c r="K58" s="5"/>
-      <c r="L58" s="5"/>
-      <c r="M58" s="5"/>
-      <c r="N58" s="5"/>
-      <c r="O58" s="4">
-        <v>1</v>
-      </c>
-      <c r="P58" s="5"/>
-      <c r="Q58" s="5"/>
-      <c r="R58" s="5"/>
-      <c r="S58" s="3"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="6"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="6"/>
+      <c r="O58" s="5">
+        <v>1</v>
+      </c>
+      <c r="P58" s="6"/>
+      <c r="Q58" s="6"/>
+      <c r="R58" s="6"/>
+      <c r="S58" s="4"/>
       <c r="T58" s="3"/>
-      <c r="U58" s="3"/>
-      <c r="V58" s="6"/>
-      <c r="W58" s="3"/>
-      <c r="X58" s="3"/>
-      <c r="Y58" s="3"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="7"/>
+      <c r="W58" s="4"/>
+      <c r="X58" s="4"/>
+      <c r="Y58" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="1" t="s">
@@ -3414,31 +3423,31 @@
       <c r="D59" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E59" s="4">
-        <v>1</v>
-      </c>
-      <c r="F59" s="4">
+      <c r="E59" s="5">
+        <v>1</v>
+      </c>
+      <c r="F59" s="5">
         <v>-1</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
-      <c r="I59" s="5"/>
-      <c r="J59" s="5"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="5"/>
-      <c r="M59" s="5"/>
-      <c r="N59" s="5"/>
-      <c r="O59" s="5"/>
-      <c r="P59" s="5"/>
-      <c r="Q59" s="5"/>
-      <c r="R59" s="5"/>
-      <c r="S59" s="3"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+      <c r="L59" s="6"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="6"/>
+      <c r="O59" s="6"/>
+      <c r="P59" s="6"/>
+      <c r="Q59" s="6"/>
+      <c r="R59" s="6"/>
+      <c r="S59" s="4"/>
       <c r="T59" s="3"/>
-      <c r="U59" s="3"/>
-      <c r="V59" s="6"/>
-      <c r="W59" s="3"/>
-      <c r="X59" s="3"/>
-      <c r="Y59" s="3"/>
+      <c r="U59" s="4"/>
+      <c r="V59" s="7"/>
+      <c r="W59" s="4"/>
+      <c r="X59" s="4"/>
+      <c r="Y59" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="1" t="s">
@@ -3453,31 +3462,31 @@
       <c r="D60" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E60" s="4">
+      <c r="E60" s="5">
         <v>3</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
-      <c r="K60" s="4">
-        <v>1</v>
-      </c>
-      <c r="L60" s="5"/>
-      <c r="M60" s="5"/>
-      <c r="N60" s="5"/>
-      <c r="O60" s="5"/>
-      <c r="P60" s="5"/>
-      <c r="Q60" s="5"/>
-      <c r="R60" s="5"/>
-      <c r="S60" s="3"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="5">
+        <v>1</v>
+      </c>
+      <c r="L60" s="6"/>
+      <c r="M60" s="6"/>
+      <c r="N60" s="6"/>
+      <c r="O60" s="6"/>
+      <c r="P60" s="6"/>
+      <c r="Q60" s="6"/>
+      <c r="R60" s="6"/>
+      <c r="S60" s="4"/>
       <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="6"/>
-      <c r="W60" s="3"/>
-      <c r="X60" s="3"/>
-      <c r="Y60" s="3"/>
+      <c r="U60" s="4"/>
+      <c r="V60" s="7"/>
+      <c r="W60" s="4"/>
+      <c r="X60" s="4"/>
+      <c r="Y60" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="1" t="s">
@@ -3492,31 +3501,31 @@
       <c r="D61" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E61" s="4">
-        <v>1</v>
-      </c>
-      <c r="F61" s="4">
+      <c r="E61" s="5">
+        <v>1</v>
+      </c>
+      <c r="F61" s="5">
         <v>1</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="5"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="5"/>
-      <c r="M61" s="5"/>
-      <c r="N61" s="5"/>
-      <c r="O61" s="5"/>
-      <c r="P61" s="5"/>
-      <c r="Q61" s="5"/>
-      <c r="R61" s="5"/>
-      <c r="S61" s="3"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="6"/>
+      <c r="O61" s="6"/>
+      <c r="P61" s="6"/>
+      <c r="Q61" s="6"/>
+      <c r="R61" s="6"/>
+      <c r="S61" s="4"/>
       <c r="T61" s="3"/>
-      <c r="U61" s="3"/>
-      <c r="V61" s="6"/>
-      <c r="W61" s="3"/>
-      <c r="X61" s="3"/>
-      <c r="Y61" s="3"/>
+      <c r="U61" s="4"/>
+      <c r="V61" s="7"/>
+      <c r="W61" s="4"/>
+      <c r="X61" s="4"/>
+      <c r="Y61" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="1" t="s">
@@ -3531,31 +3540,31 @@
       <c r="D62" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E62" s="4">
+      <c r="E62" s="5">
         <v>3</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
-      <c r="I62" s="5"/>
-      <c r="J62" s="5"/>
-      <c r="K62" s="5"/>
-      <c r="L62" s="5"/>
-      <c r="M62" s="5"/>
-      <c r="N62" s="4">
-        <v>1</v>
-      </c>
-      <c r="O62" s="5"/>
-      <c r="P62" s="5"/>
-      <c r="Q62" s="5"/>
-      <c r="R62" s="5"/>
-      <c r="S62" s="3"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="6"/>
+      <c r="N62" s="5">
+        <v>1</v>
+      </c>
+      <c r="O62" s="6"/>
+      <c r="P62" s="6"/>
+      <c r="Q62" s="6"/>
+      <c r="R62" s="6"/>
+      <c r="S62" s="4"/>
       <c r="T62" s="3"/>
-      <c r="U62" s="3"/>
-      <c r="V62" s="6"/>
-      <c r="W62" s="3"/>
-      <c r="X62" s="3"/>
-      <c r="Y62" s="3"/>
+      <c r="U62" s="4"/>
+      <c r="V62" s="7"/>
+      <c r="W62" s="4"/>
+      <c r="X62" s="4"/>
+      <c r="Y62" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="1" t="s">
@@ -3570,33 +3579,33 @@
       <c r="D63" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E63" s="4">
+      <c r="E63" s="5">
         <v>1</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
-      <c r="L63" s="4">
-        <v>1</v>
-      </c>
-      <c r="M63" s="5"/>
-      <c r="N63" s="5"/>
-      <c r="O63" s="5"/>
-      <c r="P63" s="5"/>
-      <c r="Q63" s="5"/>
-      <c r="R63" s="5"/>
-      <c r="S63" s="3" t="s">
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="5">
+        <v>1</v>
+      </c>
+      <c r="M63" s="6"/>
+      <c r="N63" s="6"/>
+      <c r="O63" s="6"/>
+      <c r="P63" s="6"/>
+      <c r="Q63" s="6"/>
+      <c r="R63" s="6"/>
+      <c r="S63" s="4" t="s">
         <v>123</v>
       </c>
       <c r="T63" s="3"/>
-      <c r="U63" s="3"/>
-      <c r="V63" s="6"/>
-      <c r="W63" s="3"/>
-      <c r="X63" s="3"/>
-      <c r="Y63" s="3"/>
+      <c r="U63" s="4"/>
+      <c r="V63" s="7"/>
+      <c r="W63" s="4"/>
+      <c r="X63" s="4"/>
+      <c r="Y63" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="1" t="s">
@@ -3611,31 +3620,31 @@
       <c r="D64" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E64" s="4">
+      <c r="E64" s="5">
         <v>2</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
-      <c r="L64" s="4">
-        <v>1</v>
-      </c>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5"/>
-      <c r="O64" s="5"/>
-      <c r="P64" s="5"/>
-      <c r="Q64" s="5"/>
-      <c r="R64" s="5"/>
-      <c r="S64" s="3"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="5">
+        <v>1</v>
+      </c>
+      <c r="M64" s="6"/>
+      <c r="N64" s="6"/>
+      <c r="O64" s="6"/>
+      <c r="P64" s="6"/>
+      <c r="Q64" s="6"/>
+      <c r="R64" s="6"/>
+      <c r="S64" s="4"/>
       <c r="T64" s="3"/>
-      <c r="U64" s="3"/>
-      <c r="V64" s="6"/>
-      <c r="W64" s="3"/>
-      <c r="X64" s="3"/>
-      <c r="Y64" s="3"/>
+      <c r="U64" s="4"/>
+      <c r="V64" s="7"/>
+      <c r="W64" s="4"/>
+      <c r="X64" s="4"/>
+      <c r="Y64" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="1" t="s">
@@ -3650,33 +3659,33 @@
       <c r="D65" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E65" s="4">
+      <c r="E65" s="5">
         <v>2</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="4">
-        <v>1</v>
-      </c>
-      <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
-      <c r="L65" s="5"/>
-      <c r="M65" s="5"/>
-      <c r="N65" s="5"/>
-      <c r="O65" s="5"/>
-      <c r="P65" s="5"/>
-      <c r="Q65" s="5"/>
-      <c r="R65" s="5"/>
-      <c r="S65" s="3" t="s">
+      <c r="H65" s="5">
+        <v>1</v>
+      </c>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="6"/>
+      <c r="O65" s="6"/>
+      <c r="P65" s="6"/>
+      <c r="Q65" s="6"/>
+      <c r="R65" s="6"/>
+      <c r="S65" s="4" t="s">
         <v>185</v>
       </c>
       <c r="T65" s="3"/>
-      <c r="U65" s="3"/>
-      <c r="V65" s="6"/>
-      <c r="W65" s="3"/>
-      <c r="X65" s="3"/>
-      <c r="Y65" s="3"/>
+      <c r="U65" s="4"/>
+      <c r="V65" s="7"/>
+      <c r="W65" s="4"/>
+      <c r="X65" s="4"/>
+      <c r="Y65" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="1" t="s">
@@ -3691,33 +3700,33 @@
       <c r="D66" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E66" s="4">
+      <c r="E66" s="5">
         <v>4</v>
       </c>
       <c r="F66" s="2"/>
-      <c r="G66" s="4">
+      <c r="G66" s="5">
         <v>-1</v>
       </c>
       <c r="H66" s="2"/>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
-      <c r="K66" s="5"/>
-      <c r="L66" s="4">
-        <v>1</v>
-      </c>
-      <c r="M66" s="5"/>
-      <c r="N66" s="5"/>
-      <c r="O66" s="5"/>
-      <c r="P66" s="5"/>
-      <c r="Q66" s="5"/>
-      <c r="R66" s="5"/>
-      <c r="S66" s="3"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="5">
+        <v>1</v>
+      </c>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
+      <c r="O66" s="6"/>
+      <c r="P66" s="6"/>
+      <c r="Q66" s="6"/>
+      <c r="R66" s="6"/>
+      <c r="S66" s="4"/>
       <c r="T66" s="3"/>
-      <c r="U66" s="3"/>
-      <c r="V66" s="6"/>
-      <c r="W66" s="3"/>
-      <c r="X66" s="3"/>
-      <c r="Y66" s="3"/>
+      <c r="U66" s="4"/>
+      <c r="V66" s="7"/>
+      <c r="W66" s="4"/>
+      <c r="X66" s="4"/>
+      <c r="Y66" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="1" t="s">
@@ -3732,37 +3741,37 @@
       <c r="D67" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E67" s="4">
+      <c r="E67" s="5">
         <v>3</v>
       </c>
-      <c r="F67" s="4">
-        <v>1</v>
-      </c>
-      <c r="G67" s="4">
+      <c r="F67" s="5">
+        <v>1</v>
+      </c>
+      <c r="G67" s="5">
         <v>1</v>
       </c>
       <c r="H67" s="2"/>
-      <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
-      <c r="M67" s="4">
-        <v>1</v>
-      </c>
-      <c r="N67" s="5"/>
-      <c r="O67" s="5"/>
-      <c r="P67" s="5"/>
-      <c r="Q67" s="5"/>
-      <c r="R67" s="5"/>
-      <c r="S67" s="3" t="s">
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="5">
+        <v>1</v>
+      </c>
+      <c r="N67" s="6"/>
+      <c r="O67" s="6"/>
+      <c r="P67" s="6"/>
+      <c r="Q67" s="6"/>
+      <c r="R67" s="6"/>
+      <c r="S67" s="4" t="s">
         <v>15</v>
       </c>
       <c r="T67" s="3"/>
-      <c r="U67" s="3"/>
-      <c r="V67" s="6"/>
-      <c r="W67" s="3"/>
-      <c r="X67" s="3"/>
-      <c r="Y67" s="3"/>
+      <c r="U67" s="4"/>
+      <c r="V67" s="7"/>
+      <c r="W67" s="4"/>
+      <c r="X67" s="4"/>
+      <c r="Y67" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="1" t="s">
@@ -3777,33 +3786,33 @@
       <c r="D68" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E68" s="4">
+      <c r="E68" s="5">
         <v>1</v>
       </c>
       <c r="F68" s="2"/>
-      <c r="G68" s="4">
+      <c r="G68" s="5">
         <v>-1</v>
       </c>
-      <c r="H68" s="4">
-        <v>1</v>
-      </c>
-      <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
-      <c r="L68" s="5"/>
-      <c r="M68" s="5"/>
-      <c r="N68" s="5"/>
-      <c r="O68" s="5"/>
-      <c r="P68" s="5"/>
-      <c r="Q68" s="5"/>
-      <c r="R68" s="5"/>
-      <c r="S68" s="3"/>
+      <c r="H68" s="5">
+        <v>1</v>
+      </c>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="6"/>
+      <c r="O68" s="6"/>
+      <c r="P68" s="6"/>
+      <c r="Q68" s="6"/>
+      <c r="R68" s="6"/>
+      <c r="S68" s="4"/>
       <c r="T68" s="3"/>
-      <c r="U68" s="3"/>
-      <c r="V68" s="6"/>
-      <c r="W68" s="3"/>
-      <c r="X68" s="3"/>
-      <c r="Y68" s="3"/>
+      <c r="U68" s="4"/>
+      <c r="V68" s="7"/>
+      <c r="W68" s="4"/>
+      <c r="X68" s="4"/>
+      <c r="Y68" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="1" t="s">
@@ -3818,33 +3827,33 @@
       <c r="D69" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E69" s="4">
+      <c r="E69" s="5">
         <v>2</v>
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="4">
-        <v>1</v>
-      </c>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
-      <c r="O69" s="5"/>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="5"/>
-      <c r="R69" s="5"/>
-      <c r="S69" s="3" t="s">
+      <c r="I69" s="6"/>
+      <c r="J69" s="5">
+        <v>1</v>
+      </c>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+      <c r="N69" s="6"/>
+      <c r="O69" s="6"/>
+      <c r="P69" s="6"/>
+      <c r="Q69" s="6"/>
+      <c r="R69" s="6"/>
+      <c r="S69" s="4" t="s">
         <v>52</v>
       </c>
       <c r="T69" s="3"/>
-      <c r="U69" s="3"/>
-      <c r="V69" s="6"/>
-      <c r="W69" s="3"/>
-      <c r="X69" s="3"/>
-      <c r="Y69" s="3"/>
+      <c r="U69" s="4"/>
+      <c r="V69" s="7"/>
+      <c r="W69" s="4"/>
+      <c r="X69" s="4"/>
+      <c r="Y69" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="1" t="s">
@@ -3859,33 +3868,33 @@
       <c r="D70" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E70" s="4">
+      <c r="E70" s="5">
         <v>2</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="4">
-        <v>1</v>
-      </c>
-      <c r="L70" s="5"/>
-      <c r="M70" s="5"/>
-      <c r="N70" s="5"/>
-      <c r="O70" s="5"/>
-      <c r="P70" s="5"/>
-      <c r="Q70" s="5"/>
-      <c r="R70" s="5"/>
-      <c r="S70" s="3" t="s">
+      <c r="I70" s="6"/>
+      <c r="J70" s="6"/>
+      <c r="K70" s="5">
+        <v>1</v>
+      </c>
+      <c r="L70" s="6"/>
+      <c r="M70" s="6"/>
+      <c r="N70" s="6"/>
+      <c r="O70" s="6"/>
+      <c r="P70" s="6"/>
+      <c r="Q70" s="6"/>
+      <c r="R70" s="6"/>
+      <c r="S70" s="4" t="s">
         <v>52</v>
       </c>
       <c r="T70" s="3"/>
-      <c r="U70" s="3"/>
-      <c r="V70" s="6"/>
-      <c r="W70" s="3"/>
-      <c r="X70" s="3"/>
-      <c r="Y70" s="3"/>
+      <c r="U70" s="4"/>
+      <c r="V70" s="7"/>
+      <c r="W70" s="4"/>
+      <c r="X70" s="4"/>
+      <c r="Y70" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="1" t="s">
@@ -3900,31 +3909,31 @@
       <c r="D71" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E71" s="4">
+      <c r="E71" s="5">
         <v>3</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
-      <c r="I71" s="5"/>
-      <c r="J71" s="4">
-        <v>1</v>
-      </c>
-      <c r="K71" s="5"/>
-      <c r="L71" s="5"/>
-      <c r="M71" s="5"/>
-      <c r="N71" s="5"/>
-      <c r="O71" s="5"/>
-      <c r="P71" s="5"/>
-      <c r="Q71" s="5"/>
-      <c r="R71" s="5"/>
-      <c r="S71" s="3"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="5">
+        <v>1</v>
+      </c>
+      <c r="K71" s="6"/>
+      <c r="L71" s="6"/>
+      <c r="M71" s="6"/>
+      <c r="N71" s="6"/>
+      <c r="O71" s="6"/>
+      <c r="P71" s="6"/>
+      <c r="Q71" s="6"/>
+      <c r="R71" s="6"/>
+      <c r="S71" s="4"/>
       <c r="T71" s="3"/>
-      <c r="U71" s="3"/>
-      <c r="V71" s="6"/>
-      <c r="W71" s="3"/>
-      <c r="X71" s="3"/>
-      <c r="Y71" s="3"/>
+      <c r="U71" s="4"/>
+      <c r="V71" s="7"/>
+      <c r="W71" s="4"/>
+      <c r="X71" s="4"/>
+      <c r="Y71" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="1" t="s">
@@ -3939,31 +3948,31 @@
       <c r="D72" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E72" s="4">
+      <c r="E72" s="5">
         <v>2</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
-      <c r="I72" s="5"/>
-      <c r="J72" s="5"/>
-      <c r="K72" s="5"/>
-      <c r="L72" s="5"/>
-      <c r="M72" s="5"/>
-      <c r="N72" s="5"/>
-      <c r="O72" s="5"/>
-      <c r="P72" s="5"/>
-      <c r="Q72" s="5"/>
-      <c r="R72" s="5"/>
-      <c r="S72" s="3" t="s">
+      <c r="I72" s="6"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="6"/>
+      <c r="M72" s="6"/>
+      <c r="N72" s="6"/>
+      <c r="O72" s="6"/>
+      <c r="P72" s="6"/>
+      <c r="Q72" s="6"/>
+      <c r="R72" s="6"/>
+      <c r="S72" s="4" t="s">
         <v>200</v>
       </c>
       <c r="T72" s="3"/>
-      <c r="U72" s="3"/>
-      <c r="V72" s="6"/>
-      <c r="W72" s="3"/>
-      <c r="X72" s="3"/>
-      <c r="Y72" s="3"/>
+      <c r="U72" s="4"/>
+      <c r="V72" s="7"/>
+      <c r="W72" s="4"/>
+      <c r="X72" s="4"/>
+      <c r="Y72" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="1" t="s">
@@ -3978,31 +3987,31 @@
       <c r="D73" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E73" s="4">
+      <c r="E73" s="5">
         <v>1</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="5"/>
-      <c r="L73" s="4">
-        <v>1</v>
-      </c>
-      <c r="M73" s="5"/>
-      <c r="N73" s="5"/>
-      <c r="O73" s="5"/>
-      <c r="P73" s="5"/>
-      <c r="Q73" s="5"/>
-      <c r="R73" s="5"/>
-      <c r="S73" s="3"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="5">
+        <v>1</v>
+      </c>
+      <c r="M73" s="6"/>
+      <c r="N73" s="6"/>
+      <c r="O73" s="6"/>
+      <c r="P73" s="6"/>
+      <c r="Q73" s="6"/>
+      <c r="R73" s="6"/>
+      <c r="S73" s="4"/>
       <c r="T73" s="3"/>
-      <c r="U73" s="3"/>
-      <c r="V73" s="6"/>
-      <c r="W73" s="3"/>
-      <c r="X73" s="3"/>
-      <c r="Y73" s="3"/>
+      <c r="U73" s="4"/>
+      <c r="V73" s="7"/>
+      <c r="W73" s="4"/>
+      <c r="X73" s="4"/>
+      <c r="Y73" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="1" t="s">
@@ -4017,33 +4026,33 @@
       <c r="D74" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E74" s="4">
+      <c r="E74" s="5">
         <v>2</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
-      <c r="M74" s="5"/>
-      <c r="N74" s="5"/>
-      <c r="O74" s="5"/>
-      <c r="P74" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q74" s="5"/>
-      <c r="R74" s="5"/>
-      <c r="S74" s="3" t="s">
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="6"/>
+      <c r="N74" s="6"/>
+      <c r="O74" s="6"/>
+      <c r="P74" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q74" s="6"/>
+      <c r="R74" s="6"/>
+      <c r="S74" s="4" t="s">
         <v>68</v>
       </c>
       <c r="T74" s="3"/>
-      <c r="U74" s="3"/>
-      <c r="V74" s="6"/>
-      <c r="W74" s="3"/>
-      <c r="X74" s="3"/>
-      <c r="Y74" s="3"/>
+      <c r="U74" s="4"/>
+      <c r="V74" s="7"/>
+      <c r="W74" s="4"/>
+      <c r="X74" s="4"/>
+      <c r="Y74" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
trigger jauge + bugs corrigés
</commit_message>
<xml_diff>
--- a/data/solutre_hex_inst.xlsx
+++ b/data/solutre_hex_inst.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mregie01\SGE\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AB6B06-EE5C-461D-A9F1-A204300AB48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Feuil1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="275">
   <si>
     <t>id</t>
   </si>
@@ -73,7 +67,7 @@
     <t>Santé</t>
   </si>
   <si>
-    <t>bouteilleBio</t>
+    <t>vinBio</t>
   </si>
   <si>
     <t>conditionAdjacence</t>
@@ -220,6 +214,9 @@
     <t>[Viticulteur,Naturaliste]</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/V13.png</t>
+  </si>
+  <si>
     <t>N1</t>
   </si>
   <si>
@@ -238,72 +235,108 @@
     <t>Restauration des murets (N)</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N1.png</t>
+  </si>
+  <si>
     <t>N3</t>
   </si>
   <si>
     <t>Restauration des murets (N2)</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N2.png</t>
+  </si>
+  <si>
     <t>N4</t>
   </si>
   <si>
     <t>Demande de subventions</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N3.png</t>
+  </si>
+  <si>
     <t>N5</t>
   </si>
   <si>
     <t>Hébergement atypique : cabane</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N4.png</t>
+  </si>
+  <si>
     <t>N6</t>
   </si>
   <si>
     <t>Atlas de la biodiversité communale</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N5.png</t>
+  </si>
+  <si>
     <t>N7</t>
   </si>
   <si>
     <t>Garde-Champêtre</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N6.png</t>
+  </si>
+  <si>
     <t>N8</t>
   </si>
   <si>
     <t>Plan de relance du bocage</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N7.png</t>
+  </si>
+  <si>
     <t>N9</t>
   </si>
   <si>
     <t>Certification forestière</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N8.png</t>
+  </si>
+  <si>
     <t>N10</t>
   </si>
   <si>
     <t>Sentier botanique</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N9.png</t>
+  </si>
+  <si>
     <t>N11</t>
   </si>
   <si>
     <t>Centre de soin de la faune sauvage</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N10.png</t>
+  </si>
+  <si>
     <t>N12</t>
   </si>
   <si>
     <t xml:space="preserve">Zone d'interdiction de la chasse et de la pêche </t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N11.png</t>
+  </si>
+  <si>
     <t>N13</t>
   </si>
   <si>
     <t>Camp de baguage d'oiseaux</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N12.png</t>
+  </si>
+  <si>
     <t>N14</t>
   </si>
   <si>
@@ -313,6 +346,9 @@
     <t>[Naturaliste,Viticulteur]</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N13.png</t>
+  </si>
+  <si>
     <t>N15</t>
   </si>
   <si>
@@ -322,6 +358,9 @@
     <t>[Naturaliste,Habitant]</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N14.png</t>
+  </si>
+  <si>
     <t>E1</t>
   </si>
   <si>
@@ -340,6 +379,9 @@
     <t>{touriste:1]</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/N15.png</t>
+  </si>
+  <si>
     <t>E2</t>
   </si>
   <si>
@@ -349,42 +391,63 @@
     <t>Tourisme</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E2.png</t>
+  </si>
+  <si>
     <t>E3</t>
   </si>
   <si>
     <t xml:space="preserve">Rénovation des logements vacants </t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E3.png</t>
+  </si>
+  <si>
     <t>E4</t>
   </si>
   <si>
     <t>Mise en place de conseils de villages</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E4.png</t>
+  </si>
+  <si>
     <t>E5</t>
   </si>
   <si>
     <t>Attribution de subventions</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E5.png</t>
+  </si>
+  <si>
     <t>E6</t>
   </si>
   <si>
     <t>Foire au vin BIO</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E6.png</t>
+  </si>
+  <si>
     <t>E7</t>
   </si>
   <si>
     <t>Création d'un Pôle d'Equilibre Territorial et Rural</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E7.png</t>
+  </si>
+  <si>
     <t>E8</t>
   </si>
   <si>
     <t>Rénovation des logements vacants 2</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E8.png</t>
+  </si>
+  <si>
     <t>E9</t>
   </si>
   <si>
@@ -394,18 +457,27 @@
     <t>Habitant</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E9.png</t>
+  </si>
+  <si>
     <t>E10</t>
   </si>
   <si>
     <t>Opération cœur de village</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E10.png</t>
+  </si>
+  <si>
     <t>E11</t>
   </si>
   <si>
     <t>Cumul de mandats</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E11.png</t>
+  </si>
+  <si>
     <t>E12</t>
   </si>
   <si>
@@ -415,6 +487,9 @@
     <t>[Elu,Naturaliste]</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E12.png</t>
+  </si>
+  <si>
     <t>E13</t>
   </si>
   <si>
@@ -424,6 +499,9 @@
     <t>[Elu,Tourisme]</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E13.png</t>
+  </si>
+  <si>
     <t>E14</t>
   </si>
   <si>
@@ -433,12 +511,18 @@
     <t>[Elu,Viticulteur]</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E14.png</t>
+  </si>
+  <si>
     <t>E15</t>
   </si>
   <si>
     <t>Placette de compostage</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/E15.png</t>
+  </si>
+  <si>
     <t>H1</t>
   </si>
   <si>
@@ -448,66 +532,99 @@
     <t>[Habitant]</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H1.png</t>
+  </si>
+  <si>
     <t>H2</t>
   </si>
   <si>
     <t>Chantier bénévole de débroussaillage</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H2.png</t>
+  </si>
+  <si>
     <t>H3</t>
   </si>
   <si>
     <t>Inventaire des vignes : Biodivine</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H3.png</t>
+  </si>
+  <si>
     <t>H4</t>
   </si>
   <si>
     <t>Mouvement démocratique local</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H4.png</t>
+  </si>
+  <si>
     <t>H5</t>
   </si>
   <si>
     <t>Chambre d'hôtes</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H5.png</t>
+  </si>
+  <si>
     <t>H6</t>
   </si>
   <si>
     <t xml:space="preserve">Sensibilisation à la biodynamie au lycée agricole </t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H6.png</t>
+  </si>
+  <si>
     <t>H7</t>
   </si>
   <si>
     <t>Lobbying associatif</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H7.png</t>
+  </si>
+  <si>
     <t>H8</t>
   </si>
   <si>
     <t xml:space="preserve">Salle de spectacles </t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H8.png</t>
+  </si>
+  <si>
     <t>H9</t>
   </si>
   <si>
     <t>Association pour le label village étoilé</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H9.png</t>
+  </si>
+  <si>
     <t>H10</t>
   </si>
   <si>
     <t>EHPAD</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H10.png</t>
+  </si>
+  <si>
     <t>H11</t>
   </si>
   <si>
     <t>Salle des fêtes</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H11.png</t>
+  </si>
+  <si>
     <t>H12</t>
   </si>
   <si>
@@ -517,18 +634,27 @@
     <t>[Habitant,Naturaliste]</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H12.png</t>
+  </si>
+  <si>
     <t>H13</t>
   </si>
   <si>
     <t>Refuge Ligue Protection des oiseaux</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H13.png</t>
+  </si>
+  <si>
     <t>H14</t>
   </si>
   <si>
     <t>Éco-pâturage</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H14.png</t>
+  </si>
+  <si>
     <t>H15</t>
   </si>
   <si>
@@ -538,6 +664,9 @@
     <t>[Habitant,Tourisme]</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/H15.png</t>
+  </si>
+  <si>
     <t>T1</t>
   </si>
   <si>
@@ -547,30 +676,45 @@
     <t>[Tourisme]</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T1.png</t>
+  </si>
+  <si>
     <t>T2</t>
   </si>
   <si>
     <t>Aérodrome/héliport</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T2.png</t>
+  </si>
+  <si>
     <t>T3</t>
   </si>
   <si>
     <t>Marché nocturne</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T3.png</t>
+  </si>
+  <si>
     <t>T4</t>
   </si>
   <si>
     <t>Mission locale</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T4.png</t>
+  </si>
+  <si>
     <t>T5</t>
   </si>
   <si>
     <t>Hôtel</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T5.png</t>
+  </si>
+  <si>
     <t>T6</t>
   </si>
   <si>
@@ -580,49 +724,70 @@
     <t>vin</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T6.png</t>
+  </si>
+  <si>
     <t>T7</t>
   </si>
   <si>
     <t>Hôtel de luxe</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T7.png</t>
+  </si>
+  <si>
     <t>T8</t>
   </si>
   <si>
     <t>Cycle de conférences sur l'écologie</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T8.png</t>
+  </si>
+  <si>
     <t>T9</t>
   </si>
   <si>
     <t>Parking Camping-Car</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T9.png</t>
+  </si>
+  <si>
     <t>T10</t>
   </si>
   <si>
     <t>Bar d'hôtel</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T10.png</t>
+  </si>
+  <si>
     <t>T11</t>
   </si>
   <si>
     <t>Brasserie</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T11.png</t>
+  </si>
+  <si>
     <t>T12</t>
   </si>
   <si>
     <t>Épicerie fine</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T12.png</t>
+  </si>
+  <si>
     <t>T13</t>
   </si>
   <si>
     <t>Woofing</t>
   </si>
   <si>
-    <t>vinBio</t>
+    <t>./icon/solutre/hex/T13.png</t>
   </si>
   <si>
     <t>T14</t>
@@ -631,6 +796,9 @@
     <t>[Tourisme,Elu]</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T14.png</t>
+  </si>
+  <si>
     <t>T15</t>
   </si>
   <si>
@@ -640,6 +808,9 @@
     <t>[Tourisme,Naturaliste]</t>
   </si>
   <si>
+    <t>./icon/solutre/hex/T15.png</t>
+  </si>
+  <si>
     <t>P1</t>
   </si>
   <si>
@@ -667,197 +838,15 @@
     <t>Caveau du plateau</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>./icon/solutre/hex/P3.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E2.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E3.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E4.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E5.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E6.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E7.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E8.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E9.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E10.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E11.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E12.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E13.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E14.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/E15.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T1.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T2.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T3.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T4.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T5.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T6.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T7.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T8.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T9.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T10.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T11.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T12.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T13.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T14.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/T15.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/V13.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N2.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N3.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H13.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H1.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H2.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H3.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H4.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H5.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H6.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H7.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H8.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H9.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H10.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H11.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H12.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H14.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/H15.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N1.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N4.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N5.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N6.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N7.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N8.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N9.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N10.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N11.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N12.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N13.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N14.png</t>
-  </si>
-  <si>
-    <t>./icon/solutre/hex/N15.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -873,13 +862,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -911,61 +900,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="14">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -976,10 +960,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -1017,71 +1001,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1109,7 +1093,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1132,11 +1116,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1145,13 +1129,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1161,7 +1145,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1170,7 +1154,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1179,7 +1163,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1187,10 +1171,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1255,42 +1239,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:Y77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y31" sqref="Y31"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.1796875" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1796875" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="11.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="14.1796875" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.54296875" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7265625" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="11.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.7265625" style="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.54296875" style="17" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.81640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28.54296875" style="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.7265625" style="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.26953125" style="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.26953125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="10" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="45.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="12" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="11" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="11" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="11" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="11" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="11" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="13" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="13" width="25.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="11" width="28.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="13" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="13" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="13" width="29.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18.75" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1367,7 +1355,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="19.5" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1401,7 +1389,7 @@
         <v>1</v>
       </c>
       <c r="S2" s="4"/>
-      <c r="T2" s="7"/>
+      <c r="T2" s="6"/>
       <c r="U2" s="4"/>
       <c r="V2" s="6"/>
       <c r="W2" s="4"/>
@@ -1410,7 +1398,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="19.5" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -1428,7 +1416,7 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="6"/>
@@ -1442,7 +1430,7 @@
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="4"/>
-      <c r="T3" s="7"/>
+      <c r="T3" s="6"/>
       <c r="U3" s="4"/>
       <c r="V3" s="6"/>
       <c r="W3" s="4"/>
@@ -1451,7 +1439,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="19.5" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -1483,7 +1471,7 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="4"/>
-      <c r="T4" s="7"/>
+      <c r="T4" s="6"/>
       <c r="U4" s="4"/>
       <c r="V4" s="6"/>
       <c r="W4" s="4"/>
@@ -1492,7 +1480,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="19.5" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
@@ -1524,7 +1512,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
       <c r="S5" s="4"/>
-      <c r="T5" s="7"/>
+      <c r="T5" s="6"/>
       <c r="U5" s="4"/>
       <c r="V5" s="6"/>
       <c r="W5" s="4"/>
@@ -1533,7 +1521,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="19.5" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -1565,7 +1553,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
       <c r="S6" s="4"/>
-      <c r="T6" s="7"/>
+      <c r="T6" s="6"/>
       <c r="U6" s="4"/>
       <c r="V6" s="6"/>
       <c r="W6" s="4"/>
@@ -1574,7 +1562,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="19.5" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -1608,7 +1596,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="S7" s="4"/>
-      <c r="T7" s="7"/>
+      <c r="T7" s="6"/>
       <c r="U7" s="4"/>
       <c r="V7" s="6"/>
       <c r="W7" s="4"/>
@@ -1617,7 +1605,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="19.5" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -1649,7 +1637,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
       <c r="S8" s="4"/>
-      <c r="T8" s="7"/>
+      <c r="T8" s="6"/>
       <c r="U8" s="4"/>
       <c r="V8" s="6"/>
       <c r="W8" s="4"/>
@@ -1658,7 +1646,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="19.5" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -1690,7 +1678,7 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="4"/>
-      <c r="T9" s="7"/>
+      <c r="T9" s="6"/>
       <c r="U9" s="4"/>
       <c r="V9" s="6"/>
       <c r="W9" s="4"/>
@@ -1699,7 +1687,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="19.5" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -1731,7 +1719,7 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="7"/>
+      <c r="T10" s="6"/>
       <c r="U10" s="4" t="s">
         <v>52</v>
       </c>
@@ -1744,7 +1732,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="19.5" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
@@ -1776,7 +1764,7 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="4"/>
-      <c r="T11" s="7"/>
+      <c r="T11" s="6"/>
       <c r="U11" s="4"/>
       <c r="V11" s="6"/>
       <c r="W11" s="4"/>
@@ -1785,7 +1773,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="19.5" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>57</v>
       </c>
@@ -1817,7 +1805,7 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="4"/>
-      <c r="T12" s="7"/>
+      <c r="T12" s="6"/>
       <c r="U12" s="4"/>
       <c r="V12" s="6"/>
       <c r="W12" s="4"/>
@@ -1826,7 +1814,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="19.5" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>60</v>
       </c>
@@ -1858,7 +1846,7 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="4"/>
-      <c r="T13" s="7"/>
+      <c r="T13" s="6"/>
       <c r="U13" s="4"/>
       <c r="V13" s="6"/>
       <c r="W13" s="4"/>
@@ -1867,7 +1855,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="19.5" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
         <v>63</v>
       </c>
@@ -1899,27 +1887,27 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="4"/>
-      <c r="T14" s="7"/>
+      <c r="T14" s="6"/>
       <c r="U14" s="4"/>
       <c r="V14" s="6"/>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
       <c r="Y14" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="19.5" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E15" s="5">
         <v>3</v>
@@ -1946,27 +1934,27 @@
       <c r="S15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T15" s="7"/>
+      <c r="T15" s="6"/>
       <c r="U15" s="4"/>
       <c r="V15" s="6"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
       <c r="Y15" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="19.5" customHeight="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="E16" s="5">
         <v>3</v>
@@ -1987,27 +1975,27 @@
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="4"/>
-      <c r="T16" s="7"/>
+      <c r="T16" s="6"/>
       <c r="U16" s="4"/>
       <c r="V16" s="6"/>
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
-      <c r="Y16" s="16" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" ht="19.5" customHeight="1">
+      <c r="Y16" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E17" s="5">
         <v>1</v>
@@ -2026,27 +2014,27 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="4"/>
-      <c r="T17" s="7"/>
+      <c r="T17" s="6"/>
       <c r="U17" s="4"/>
       <c r="V17" s="6"/>
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
       <c r="Y17" s="4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" ht="19.5" customHeight="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E18" s="5">
         <v>2</v>
@@ -2065,27 +2053,27 @@
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
       <c r="S18" s="4"/>
-      <c r="T18" s="7"/>
+      <c r="T18" s="6"/>
       <c r="U18" s="4"/>
       <c r="V18" s="6"/>
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
       <c r="Y18" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" ht="19.5" customHeight="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E19" s="5">
         <v>2</v>
@@ -2106,27 +2094,27 @@
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
       <c r="S19" s="4"/>
-      <c r="T19" s="7"/>
+      <c r="T19" s="6"/>
       <c r="U19" s="4"/>
       <c r="V19" s="6"/>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
       <c r="Y19" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" ht="19.5" customHeight="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E20" s="5">
         <v>2</v>
@@ -2147,27 +2135,27 @@
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="4"/>
-      <c r="T20" s="7"/>
+      <c r="T20" s="6"/>
       <c r="U20" s="4"/>
       <c r="V20" s="6"/>
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" ht="19.5" customHeight="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E21" s="5">
         <v>1</v>
@@ -2186,27 +2174,27 @@
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="4"/>
-      <c r="T21" s="7"/>
+      <c r="T21" s="6"/>
       <c r="U21" s="4"/>
       <c r="V21" s="6"/>
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
       <c r="Y21" s="4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" ht="19.5" customHeight="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
@@ -2225,27 +2213,27 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="4"/>
-      <c r="T22" s="7"/>
+      <c r="T22" s="6"/>
       <c r="U22" s="4"/>
       <c r="V22" s="6"/>
       <c r="W22" s="4"/>
       <c r="X22" s="4"/>
       <c r="Y22" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" ht="19.5" customHeight="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E23" s="5">
         <v>3</v>
@@ -2266,27 +2254,27 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="4"/>
-      <c r="T23" s="7"/>
+      <c r="T23" s="6"/>
       <c r="U23" s="4"/>
       <c r="V23" s="6"/>
       <c r="W23" s="4"/>
       <c r="X23" s="4"/>
       <c r="Y23" s="4" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" ht="19.5" customHeight="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E24" s="5">
         <v>3</v>
@@ -2307,27 +2295,27 @@
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
       <c r="S24" s="4"/>
-      <c r="T24" s="7"/>
+      <c r="T24" s="6"/>
       <c r="U24" s="4"/>
       <c r="V24" s="6"/>
       <c r="W24" s="4"/>
       <c r="X24" s="4"/>
       <c r="Y24" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" ht="19.5" customHeight="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
@@ -2348,27 +2336,27 @@
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
       <c r="S25" s="4"/>
-      <c r="T25" s="7"/>
+      <c r="T25" s="6"/>
       <c r="U25" s="4"/>
       <c r="V25" s="6"/>
       <c r="W25" s="4"/>
       <c r="X25" s="4"/>
       <c r="Y25" s="4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" ht="19.5" customHeight="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E26" s="5">
         <v>1</v>
@@ -2393,27 +2381,27 @@
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
       <c r="S26" s="4"/>
-      <c r="T26" s="7"/>
+      <c r="T26" s="6"/>
       <c r="U26" s="4"/>
       <c r="V26" s="6"/>
       <c r="W26" s="4"/>
       <c r="X26" s="4"/>
       <c r="Y26" s="4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" ht="19.5" customHeight="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E27" s="5">
         <v>1</v>
@@ -2434,27 +2422,27 @@
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
       <c r="S27" s="4"/>
-      <c r="T27" s="7"/>
+      <c r="T27" s="6"/>
       <c r="U27" s="4"/>
       <c r="V27" s="6"/>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
       <c r="Y27" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" ht="19.5" customHeight="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="E28" s="5">
         <v>3</v>
@@ -2475,27 +2463,27 @@
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
       <c r="S28" s="4"/>
-      <c r="T28" s="7"/>
+      <c r="T28" s="6"/>
       <c r="U28" s="4"/>
       <c r="V28" s="6"/>
       <c r="W28" s="4"/>
       <c r="X28" s="4"/>
       <c r="Y28" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" ht="19.5" customHeight="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E29" s="5">
         <v>2</v>
@@ -2516,27 +2504,27 @@
       <c r="S29" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T29" s="7"/>
+      <c r="T29" s="6"/>
       <c r="U29" s="4"/>
       <c r="V29" s="6"/>
       <c r="W29" s="4"/>
       <c r="X29" s="4"/>
       <c r="Y29" s="4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" ht="19.5" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E30" s="5">
         <v>2</v>
@@ -2557,31 +2545,31 @@
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
       <c r="S30" s="4"/>
-      <c r="T30" s="7"/>
+      <c r="T30" s="6"/>
       <c r="U30" s="4"/>
       <c r="V30" s="6"/>
       <c r="W30" s="1" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="X30" s="1" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" ht="19.5" customHeight="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E31" s="5">
         <v>3</v>
@@ -2602,29 +2590,29 @@
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
       <c r="S31" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="T31" s="7"/>
+        <v>124</v>
+      </c>
+      <c r="T31" s="6"/>
       <c r="U31" s="4"/>
       <c r="V31" s="6"/>
       <c r="W31" s="4"/>
       <c r="X31" s="4"/>
       <c r="Y31" s="4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" ht="19.5" customHeight="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="1" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E32" s="5">
         <v>3</v>
@@ -2645,27 +2633,27 @@
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
       <c r="S32" s="4"/>
-      <c r="T32" s="7"/>
+      <c r="T32" s="6"/>
       <c r="U32" s="4"/>
       <c r="V32" s="6"/>
       <c r="W32" s="4"/>
       <c r="X32" s="4"/>
       <c r="Y32" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" ht="19.5" customHeight="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="1" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E33" s="5">
         <v>2</v>
@@ -2686,27 +2674,27 @@
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
       <c r="S33" s="4"/>
-      <c r="T33" s="7"/>
+      <c r="T33" s="6"/>
       <c r="U33" s="4"/>
       <c r="V33" s="6"/>
       <c r="W33" s="4"/>
       <c r="X33" s="4"/>
       <c r="Y33" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25" ht="19.5" customHeight="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="1" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E34" s="5">
         <v>1</v>
@@ -2725,27 +2713,27 @@
       <c r="Q34" s="6"/>
       <c r="R34" s="6"/>
       <c r="S34" s="4"/>
-      <c r="T34" s="7"/>
+      <c r="T34" s="6"/>
       <c r="U34" s="4"/>
       <c r="V34" s="6"/>
       <c r="W34" s="4"/>
       <c r="X34" s="4"/>
       <c r="Y34" s="4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25" ht="19.5" customHeight="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="1" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E35" s="5">
         <v>2</v>
@@ -2766,27 +2754,27 @@
       <c r="Q35" s="6"/>
       <c r="R35" s="6"/>
       <c r="S35" s="4"/>
-      <c r="T35" s="7"/>
+      <c r="T35" s="6"/>
       <c r="U35" s="4"/>
       <c r="V35" s="6"/>
       <c r="W35" s="4"/>
       <c r="X35" s="4"/>
       <c r="Y35" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" ht="19.5" customHeight="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="E36" s="5">
         <v>3</v>
@@ -2805,27 +2793,27 @@
       <c r="Q36" s="6"/>
       <c r="R36" s="6"/>
       <c r="S36" s="4"/>
-      <c r="T36" s="7"/>
+      <c r="T36" s="6"/>
       <c r="U36" s="4"/>
       <c r="V36" s="6"/>
       <c r="W36" s="4"/>
       <c r="X36" s="4"/>
       <c r="Y36" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" ht="19.5" customHeight="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="1" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E37" s="5">
         <v>3</v>
@@ -2846,27 +2834,27 @@
       <c r="Q37" s="6"/>
       <c r="R37" s="6"/>
       <c r="S37" s="4"/>
-      <c r="T37" s="7"/>
+      <c r="T37" s="6"/>
       <c r="U37" s="4"/>
       <c r="V37" s="6"/>
       <c r="W37" s="4"/>
       <c r="X37" s="4"/>
       <c r="Y37" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25" ht="19.5" customHeight="1">
+        <v>143</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="1" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E38" s="5">
         <v>3</v>
@@ -2891,7 +2879,7 @@
       </c>
       <c r="R38" s="6"/>
       <c r="S38" s="4" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="T38" s="6">
         <v>2</v>
@@ -2901,21 +2889,21 @@
       <c r="W38" s="4"/>
       <c r="X38" s="4"/>
       <c r="Y38" s="4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25" ht="19.5" customHeight="1">
+        <v>147</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="1" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E39" s="5">
         <v>2</v>
@@ -2936,27 +2924,27 @@
       <c r="Q39" s="6"/>
       <c r="R39" s="6"/>
       <c r="S39" s="4"/>
-      <c r="T39" s="7"/>
+      <c r="T39" s="6"/>
       <c r="U39" s="4"/>
       <c r="V39" s="6"/>
       <c r="W39" s="4"/>
       <c r="X39" s="4"/>
       <c r="Y39" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25" ht="19.5" customHeight="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="1" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E40" s="5">
         <v>2</v>
@@ -2975,27 +2963,27 @@
       <c r="Q40" s="6"/>
       <c r="R40" s="6"/>
       <c r="S40" s="4"/>
-      <c r="T40" s="7"/>
+      <c r="T40" s="6"/>
       <c r="U40" s="4"/>
       <c r="V40" s="6"/>
       <c r="W40" s="4"/>
       <c r="X40" s="4"/>
       <c r="Y40" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" ht="19.5" customHeight="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="1" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="E41" s="5">
         <v>2</v>
@@ -3014,27 +3002,27 @@
       <c r="Q41" s="6"/>
       <c r="R41" s="6"/>
       <c r="S41" s="4"/>
-      <c r="T41" s="7"/>
+      <c r="T41" s="6"/>
       <c r="U41" s="4"/>
       <c r="V41" s="6"/>
       <c r="W41" s="4"/>
       <c r="X41" s="4"/>
       <c r="Y41" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" ht="19.5" customHeight="1">
+        <v>157</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="1" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="E42" s="5">
         <v>1</v>
@@ -3055,27 +3043,27 @@
       <c r="Q42" s="6"/>
       <c r="R42" s="6"/>
       <c r="S42" s="4"/>
-      <c r="T42" s="7"/>
+      <c r="T42" s="6"/>
       <c r="U42" s="4"/>
       <c r="V42" s="6"/>
       <c r="W42" s="4"/>
       <c r="X42" s="4"/>
       <c r="Y42" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" ht="19.5" customHeight="1">
+        <v>161</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="1" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="E43" s="5">
         <v>2</v>
@@ -3094,27 +3082,27 @@
       <c r="Q43" s="6"/>
       <c r="R43" s="6"/>
       <c r="S43" s="4"/>
-      <c r="T43" s="7"/>
+      <c r="T43" s="6"/>
       <c r="U43" s="4"/>
       <c r="V43" s="6"/>
       <c r="W43" s="4"/>
       <c r="X43" s="4"/>
       <c r="Y43" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" ht="19.5" customHeight="1">
+        <v>165</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="1" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="E44" s="5">
         <v>2</v>
@@ -3135,29 +3123,29 @@
       <c r="Q44" s="6"/>
       <c r="R44" s="6"/>
       <c r="S44" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="T44" s="7"/>
+        <v>146</v>
+      </c>
+      <c r="T44" s="6"/>
       <c r="U44" s="4"/>
       <c r="V44" s="6"/>
       <c r="W44" s="4"/>
       <c r="X44" s="4"/>
       <c r="Y44" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="45" spans="1:25" ht="19.5" customHeight="1">
+        <v>168</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="1" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E45" s="5">
         <v>1</v>
@@ -3176,27 +3164,27 @@
       <c r="Q45" s="6"/>
       <c r="R45" s="6"/>
       <c r="S45" s="4"/>
-      <c r="T45" s="7"/>
+      <c r="T45" s="6"/>
       <c r="U45" s="4"/>
       <c r="V45" s="6"/>
       <c r="W45" s="4"/>
       <c r="X45" s="4"/>
       <c r="Y45" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" ht="19.5" customHeight="1">
+        <v>172</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="1" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>143</v>
+        <v>174</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E46" s="5">
         <v>2</v>
@@ -3215,29 +3203,29 @@
       <c r="Q46" s="6"/>
       <c r="R46" s="6"/>
       <c r="S46" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="T46" s="7"/>
+        <v>69</v>
+      </c>
+      <c r="T46" s="6"/>
       <c r="U46" s="4"/>
       <c r="V46" s="6"/>
       <c r="W46" s="4"/>
       <c r="X46" s="4"/>
       <c r="Y46" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="47" spans="1:25" ht="19.5" customHeight="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="1" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E47" s="5">
         <v>2</v>
@@ -3256,27 +3244,27 @@
       <c r="Q47" s="6"/>
       <c r="R47" s="6"/>
       <c r="S47" s="4"/>
-      <c r="T47" s="7"/>
+      <c r="T47" s="6"/>
       <c r="U47" s="4"/>
       <c r="V47" s="6"/>
       <c r="W47" s="4"/>
       <c r="X47" s="4"/>
       <c r="Y47" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" ht="19.5" customHeight="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="D48" s="1" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E48" s="5">
         <v>3</v>
@@ -3297,27 +3285,27 @@
       <c r="Q48" s="6"/>
       <c r="R48" s="6"/>
       <c r="S48" s="4"/>
-      <c r="T48" s="7"/>
+      <c r="T48" s="6"/>
       <c r="U48" s="4"/>
       <c r="V48" s="6"/>
       <c r="W48" s="4"/>
       <c r="X48" s="4"/>
       <c r="Y48" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" ht="19.5" customHeight="1">
+        <v>181</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="1" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E49" s="5">
         <v>3</v>
@@ -3336,27 +3324,27 @@
       <c r="Q49" s="6"/>
       <c r="R49" s="6"/>
       <c r="S49" s="4"/>
-      <c r="T49" s="7"/>
+      <c r="T49" s="6"/>
       <c r="U49" s="4"/>
       <c r="V49" s="6"/>
       <c r="W49" s="4"/>
       <c r="X49" s="4"/>
       <c r="Y49" s="4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="50" spans="1:25" ht="19.5" customHeight="1">
+        <v>184</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="1" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E50" s="5">
         <v>2</v>
@@ -3377,27 +3365,27 @@
       <c r="Q50" s="6"/>
       <c r="R50" s="6"/>
       <c r="S50" s="4"/>
-      <c r="T50" s="7"/>
+      <c r="T50" s="6"/>
       <c r="U50" s="4"/>
       <c r="V50" s="6"/>
       <c r="W50" s="4"/>
       <c r="X50" s="4"/>
       <c r="Y50" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" ht="19.5" customHeight="1">
+        <v>187</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="1" t="s">
-        <v>152</v>
+        <v>188</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E51" s="5">
         <v>2</v>
@@ -3418,27 +3406,27 @@
       <c r="Q51" s="6"/>
       <c r="R51" s="6"/>
       <c r="S51" s="4"/>
-      <c r="T51" s="7"/>
+      <c r="T51" s="6"/>
       <c r="U51" s="4"/>
       <c r="V51" s="6"/>
       <c r="W51" s="4"/>
       <c r="X51" s="4"/>
       <c r="Y51" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" ht="19.5" customHeight="1">
+        <v>190</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="1" t="s">
-        <v>154</v>
+        <v>191</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>155</v>
+        <v>192</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E52" s="5">
         <v>2</v>
@@ -3457,27 +3445,27 @@
       <c r="Q52" s="6"/>
       <c r="R52" s="6"/>
       <c r="S52" s="4"/>
-      <c r="T52" s="7"/>
+      <c r="T52" s="6"/>
       <c r="U52" s="4"/>
       <c r="V52" s="6"/>
       <c r="W52" s="4"/>
       <c r="X52" s="4"/>
       <c r="Y52" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="53" spans="1:25" ht="19.5" customHeight="1">
+        <v>193</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="1" t="s">
-        <v>156</v>
+        <v>194</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E53" s="5">
         <v>3</v>
@@ -3496,27 +3484,27 @@
       <c r="Q53" s="6"/>
       <c r="R53" s="6"/>
       <c r="S53" s="4"/>
-      <c r="T53" s="7"/>
+      <c r="T53" s="6"/>
       <c r="U53" s="4"/>
       <c r="V53" s="6"/>
       <c r="W53" s="4"/>
       <c r="X53" s="4"/>
       <c r="Y53" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25" ht="19.5" customHeight="1">
+        <v>196</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="1" t="s">
-        <v>158</v>
+        <v>197</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>159</v>
+        <v>198</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E54" s="5">
         <v>2</v>
@@ -3541,27 +3529,27 @@
       </c>
       <c r="R54" s="6"/>
       <c r="S54" s="4"/>
-      <c r="T54" s="7"/>
+      <c r="T54" s="6"/>
       <c r="U54" s="4"/>
       <c r="V54" s="6"/>
       <c r="W54" s="4"/>
       <c r="X54" s="4"/>
       <c r="Y54" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25" ht="18.75" customHeight="1">
+        <v>199</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="1" t="s">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>161</v>
+        <v>201</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="E55" s="5">
         <v>2</v>
@@ -3584,27 +3572,27 @@
       <c r="Q55" s="6"/>
       <c r="R55" s="6"/>
       <c r="S55" s="4"/>
-      <c r="T55" s="7"/>
+      <c r="T55" s="6"/>
       <c r="U55" s="4"/>
       <c r="V55" s="6"/>
       <c r="W55" s="4"/>
       <c r="X55" s="4"/>
       <c r="Y55" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="56" spans="1:25" ht="18.75" customHeight="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="1" t="s">
-        <v>162</v>
+        <v>203</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>163</v>
+        <v>204</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>164</v>
+        <v>205</v>
       </c>
       <c r="E56" s="5">
         <v>3</v>
@@ -3629,29 +3617,29 @@
       <c r="Q56" s="6"/>
       <c r="R56" s="6"/>
       <c r="S56" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="T56" s="7"/>
+        <v>69</v>
+      </c>
+      <c r="T56" s="6"/>
       <c r="U56" s="4"/>
       <c r="V56" s="6"/>
       <c r="W56" s="4"/>
       <c r="X56" s="4"/>
       <c r="Y56" s="4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="57" spans="1:25" ht="18.75" customHeight="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="1" t="s">
-        <v>165</v>
+        <v>207</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>166</v>
+        <v>208</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>164</v>
+        <v>205</v>
       </c>
       <c r="E57" s="5">
         <v>2</v>
@@ -3670,29 +3658,29 @@
       <c r="Q57" s="6"/>
       <c r="R57" s="6"/>
       <c r="S57" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="T57" s="7"/>
+        <v>69</v>
+      </c>
+      <c r="T57" s="6"/>
       <c r="U57" s="4"/>
       <c r="V57" s="6"/>
       <c r="W57" s="4"/>
       <c r="X57" s="4"/>
       <c r="Y57" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="58" spans="1:25" ht="18.75" customHeight="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="1" t="s">
-        <v>167</v>
+        <v>210</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>168</v>
+        <v>211</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>164</v>
+        <v>205</v>
       </c>
       <c r="E58" s="5">
         <v>3</v>
@@ -3713,27 +3701,27 @@
       <c r="Q58" s="6"/>
       <c r="R58" s="6"/>
       <c r="S58" s="4"/>
-      <c r="T58" s="7"/>
+      <c r="T58" s="6"/>
       <c r="U58" s="4"/>
       <c r="V58" s="6"/>
       <c r="W58" s="4"/>
       <c r="X58" s="4"/>
       <c r="Y58" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="59" spans="1:25" ht="18.75" customHeight="1">
+        <v>212</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="1" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>170</v>
+        <v>214</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>171</v>
+        <v>215</v>
       </c>
       <c r="E59" s="5">
         <v>1</v>
@@ -3754,27 +3742,27 @@
       <c r="Q59" s="6"/>
       <c r="R59" s="6"/>
       <c r="S59" s="4"/>
-      <c r="T59" s="7"/>
+      <c r="T59" s="6"/>
       <c r="U59" s="4"/>
       <c r="V59" s="6"/>
       <c r="W59" s="4"/>
       <c r="X59" s="4"/>
       <c r="Y59" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="60" spans="1:25" ht="18.75" customHeight="1">
+        <v>216</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="1" t="s">
-        <v>172</v>
+        <v>217</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>173</v>
+        <v>218</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E60" s="5">
         <v>3</v>
@@ -3795,27 +3783,27 @@
       <c r="Q60" s="6"/>
       <c r="R60" s="6"/>
       <c r="S60" s="4"/>
-      <c r="T60" s="7"/>
+      <c r="T60" s="6"/>
       <c r="U60" s="4"/>
       <c r="V60" s="6"/>
       <c r="W60" s="4"/>
       <c r="X60" s="4"/>
       <c r="Y60" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="61" spans="1:25" ht="18.75" customHeight="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="1" t="s">
-        <v>175</v>
+        <v>221</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>176</v>
+        <v>222</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E61" s="5">
         <v>1</v>
@@ -3836,27 +3824,27 @@
       <c r="Q61" s="6"/>
       <c r="R61" s="6"/>
       <c r="S61" s="4"/>
-      <c r="T61" s="7"/>
+      <c r="T61" s="6"/>
       <c r="U61" s="4"/>
       <c r="V61" s="6"/>
       <c r="W61" s="4"/>
       <c r="X61" s="4"/>
       <c r="Y61" s="4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="62" spans="1:25" ht="18.75" customHeight="1">
+        <v>223</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="1" t="s">
-        <v>177</v>
+        <v>224</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>178</v>
+        <v>225</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E62" s="5">
         <v>3</v>
@@ -3877,27 +3865,27 @@
       <c r="Q62" s="6"/>
       <c r="R62" s="6"/>
       <c r="S62" s="4"/>
-      <c r="T62" s="7"/>
+      <c r="T62" s="6"/>
       <c r="U62" s="4"/>
       <c r="V62" s="6"/>
       <c r="W62" s="4"/>
       <c r="X62" s="4"/>
       <c r="Y62" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="63" spans="1:25" ht="18.75" customHeight="1">
+        <v>226</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="1" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>180</v>
+        <v>228</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E63" s="5">
         <v>1</v>
@@ -3918,29 +3906,29 @@
       <c r="Q63" s="6"/>
       <c r="R63" s="6"/>
       <c r="S63" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="T63" s="7"/>
+        <v>146</v>
+      </c>
+      <c r="T63" s="6"/>
       <c r="U63" s="4"/>
       <c r="V63" s="6"/>
       <c r="W63" s="4"/>
       <c r="X63" s="4"/>
       <c r="Y63" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="64" spans="1:25" ht="18.75" customHeight="1">
+        <v>229</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="1" t="s">
-        <v>181</v>
+        <v>230</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>182</v>
+        <v>231</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E64" s="5">
         <v>2</v>
@@ -3961,27 +3949,27 @@
       <c r="Q64" s="6"/>
       <c r="R64" s="6"/>
       <c r="S64" s="4"/>
-      <c r="T64" s="7"/>
+      <c r="T64" s="6"/>
       <c r="U64" s="4"/>
       <c r="V64" s="6"/>
       <c r="W64" s="4"/>
       <c r="X64" s="4"/>
       <c r="Y64" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="65" spans="1:25" ht="18.75" customHeight="1">
+        <v>232</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="1" t="s">
-        <v>183</v>
+        <v>233</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>184</v>
+        <v>234</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E65" s="5">
         <v>2</v>
@@ -4002,9 +3990,9 @@
       <c r="Q65" s="6"/>
       <c r="R65" s="6"/>
       <c r="S65" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="T65" s="7"/>
+        <v>235</v>
+      </c>
+      <c r="T65" s="6"/>
       <c r="U65" s="4"/>
       <c r="V65" s="6"/>
       <c r="W65" s="4"/>
@@ -4013,18 +4001,18 @@
         <v>236</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="18.75" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="1" t="s">
-        <v>186</v>
+        <v>237</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>187</v>
+        <v>238</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E66" s="5">
         <v>4</v>
@@ -4047,27 +4035,27 @@
       <c r="Q66" s="6"/>
       <c r="R66" s="6"/>
       <c r="S66" s="4"/>
-      <c r="T66" s="7"/>
+      <c r="T66" s="6"/>
       <c r="U66" s="4"/>
       <c r="V66" s="6"/>
       <c r="W66" s="4"/>
       <c r="X66" s="4"/>
       <c r="Y66" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="67" spans="1:25" ht="18.75" customHeight="1">
+        <v>239</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="1" t="s">
-        <v>188</v>
+        <v>240</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>189</v>
+        <v>241</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E67" s="5">
         <v>3</v>
@@ -4094,27 +4082,27 @@
       <c r="S67" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="T67" s="7"/>
+      <c r="T67" s="6"/>
       <c r="U67" s="4"/>
       <c r="V67" s="6"/>
       <c r="W67" s="4"/>
       <c r="X67" s="4"/>
       <c r="Y67" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="68" spans="1:25" ht="18.75" customHeight="1">
+        <v>242</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="1" t="s">
-        <v>190</v>
+        <v>243</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>191</v>
+        <v>244</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E68" s="5">
         <v>1</v>
@@ -4137,27 +4125,27 @@
       <c r="Q68" s="6"/>
       <c r="R68" s="6"/>
       <c r="S68" s="4"/>
-      <c r="T68" s="7"/>
+      <c r="T68" s="6"/>
       <c r="U68" s="4"/>
       <c r="V68" s="6"/>
       <c r="W68" s="4"/>
       <c r="X68" s="4"/>
       <c r="Y68" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="69" spans="1:25" ht="18.75" customHeight="1">
+        <v>245</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="1" t="s">
-        <v>192</v>
+        <v>246</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>193</v>
+        <v>247</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E69" s="5">
         <v>2</v>
@@ -4180,27 +4168,27 @@
       <c r="S69" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="T69" s="7"/>
+      <c r="T69" s="6"/>
       <c r="U69" s="4"/>
       <c r="V69" s="6"/>
       <c r="W69" s="4"/>
       <c r="X69" s="4"/>
       <c r="Y69" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="70" spans="1:25" ht="18.75" customHeight="1">
+        <v>248</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="1" t="s">
-        <v>194</v>
+        <v>249</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>195</v>
+        <v>250</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E70" s="5">
         <v>2</v>
@@ -4223,27 +4211,27 @@
       <c r="S70" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="T70" s="7"/>
+      <c r="T70" s="6"/>
       <c r="U70" s="4"/>
       <c r="V70" s="6"/>
       <c r="W70" s="4"/>
       <c r="X70" s="4"/>
       <c r="Y70" s="4" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="71" spans="1:25" ht="18.75" customHeight="1">
+        <v>251</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="1" t="s">
-        <v>196</v>
+        <v>252</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>197</v>
+        <v>253</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E71" s="5">
         <v>3</v>
@@ -4264,27 +4252,27 @@
       <c r="Q71" s="6"/>
       <c r="R71" s="6"/>
       <c r="S71" s="4"/>
-      <c r="T71" s="7"/>
+      <c r="T71" s="6"/>
       <c r="U71" s="4"/>
       <c r="V71" s="6"/>
       <c r="W71" s="4"/>
       <c r="X71" s="4"/>
       <c r="Y71" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="72" spans="1:25" ht="18.75" customHeight="1">
+        <v>254</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="1" t="s">
-        <v>198</v>
+        <v>255</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>199</v>
+        <v>256</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>174</v>
+        <v>219</v>
       </c>
       <c r="E72" s="5">
         <v>2</v>
@@ -4303,29 +4291,29 @@
       <c r="Q72" s="6"/>
       <c r="R72" s="6"/>
       <c r="S72" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="T72" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="T72" s="6"/>
       <c r="U72" s="4"/>
       <c r="V72" s="6"/>
       <c r="W72" s="4"/>
       <c r="X72" s="4"/>
       <c r="Y72" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="73" spans="1:25" ht="18.75" customHeight="1">
+        <v>257</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="1" t="s">
-        <v>201</v>
+        <v>258</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>202</v>
+        <v>259</v>
       </c>
       <c r="E73" s="5">
         <v>1</v>
@@ -4346,27 +4334,27 @@
       <c r="Q73" s="6"/>
       <c r="R73" s="6"/>
       <c r="S73" s="4"/>
-      <c r="T73" s="7"/>
+      <c r="T73" s="6"/>
       <c r="U73" s="4"/>
       <c r="V73" s="6"/>
       <c r="W73" s="4"/>
       <c r="X73" s="4"/>
       <c r="Y73" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="74" spans="1:25" ht="18.75" customHeight="1">
+        <v>260</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="1" t="s">
-        <v>203</v>
+        <v>261</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>204</v>
+        <v>262</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>205</v>
+        <v>263</v>
       </c>
       <c r="E74" s="5">
         <v>2</v>
@@ -4387,107 +4375,107 @@
       <c r="Q74" s="6"/>
       <c r="R74" s="6"/>
       <c r="S74" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="T74" s="7"/>
+        <v>69</v>
+      </c>
+      <c r="T74" s="6"/>
       <c r="U74" s="4"/>
       <c r="V74" s="6"/>
       <c r="W74" s="4"/>
       <c r="X74" s="4"/>
-      <c r="Y74" s="16" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="75" spans="1:25" ht="18.75" customHeight="1">
-      <c r="A75" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="E75" s="9">
+      <c r="Y74" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+      <c r="A75" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E75" s="8">
         <v>0</v>
       </c>
-      <c r="F75" s="10"/>
-      <c r="G75" s="10"/>
-      <c r="H75" s="10"/>
-      <c r="I75" s="9"/>
-      <c r="J75" s="9"/>
-      <c r="K75" s="9"/>
-      <c r="L75" s="9"/>
-      <c r="M75" s="9"/>
-      <c r="N75" s="9"/>
-      <c r="O75" s="9"/>
-      <c r="P75" s="9"/>
-      <c r="Q75" s="9"/>
-      <c r="R75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="8"/>
+      <c r="K75" s="8"/>
+      <c r="L75" s="8"/>
+      <c r="M75" s="8"/>
+      <c r="N75" s="8"/>
+      <c r="O75" s="8"/>
+      <c r="P75" s="8"/>
+      <c r="Q75" s="8"/>
+      <c r="R75" s="8"/>
       <c r="S75" s="4"/>
-      <c r="T75" s="11"/>
+      <c r="T75" s="8"/>
       <c r="U75" s="4"/>
-      <c r="V75" s="9"/>
+      <c r="V75" s="8"/>
       <c r="W75" s="4"/>
       <c r="X75" s="4"/>
       <c r="Y75" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="76" spans="1:25" ht="18.75" customHeight="1">
-      <c r="A76" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C76" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+      <c r="A76" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C76" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D76" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="E76" s="9">
+      <c r="D76" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E76" s="8">
         <v>0</v>
       </c>
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
-      <c r="H76" s="10"/>
-      <c r="I76" s="9"/>
-      <c r="J76" s="9"/>
-      <c r="K76" s="9"/>
-      <c r="L76" s="9"/>
-      <c r="M76" s="9"/>
-      <c r="N76" s="9"/>
-      <c r="O76" s="9"/>
-      <c r="P76" s="9"/>
-      <c r="Q76" s="9"/>
-      <c r="R76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="8"/>
+      <c r="J76" s="8"/>
+      <c r="K76" s="8"/>
+      <c r="L76" s="8"/>
+      <c r="M76" s="8"/>
+      <c r="N76" s="8"/>
+      <c r="O76" s="8"/>
+      <c r="P76" s="8"/>
+      <c r="Q76" s="8"/>
+      <c r="R76" s="8"/>
       <c r="S76" s="4"/>
-      <c r="T76" s="11"/>
+      <c r="T76" s="8"/>
       <c r="U76" s="4"/>
-      <c r="V76" s="9"/>
+      <c r="V76" s="8"/>
       <c r="W76" s="4"/>
       <c r="X76" s="4"/>
       <c r="Y76" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="77" spans="1:25" ht="18.75" customHeight="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="1" t="s">
-        <v>213</v>
+        <v>272</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>214</v>
+        <v>273</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>208</v>
+        <v>267</v>
       </c>
       <c r="E77" s="5">
         <v>0</v>
@@ -4505,16 +4493,14 @@
       <c r="P77" s="5"/>
       <c r="Q77" s="6"/>
       <c r="R77" s="6"/>
-      <c r="S77" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="T77" s="7"/>
+      <c r="S77" s="4"/>
+      <c r="T77" s="6"/>
       <c r="U77" s="4"/>
       <c r="V77" s="6"/>
       <c r="W77" s="4"/>
       <c r="X77" s="4"/>
       <c r="Y77" s="4" t="s">
-        <v>216</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>